<commit_message>
big update with working from_df and weighted dissimilarity
</commit_message>
<xml_diff>
--- a/data/input/example_usage.xlsx
+++ b/data/input/example_usage.xlsx
@@ -8542,10 +8542,10 @@
         <v>10.2735</v>
       </c>
       <c r="C2" t="n">
-        <v>46.33333333333334</v>
+        <v>51.16666666666666</v>
       </c>
       <c r="D2" t="n">
-        <v>55.33333333333334</v>
+        <v>37.16666666666666</v>
       </c>
       <c r="E2" t="n">
         <v>6</v>
@@ -8562,10 +8562,10 @@
         <v>9.667249999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>20.5</v>
+        <v>57.75</v>
       </c>
       <c r="D3" t="n">
-        <v>76.75</v>
+        <v>28.75</v>
       </c>
       <c r="E3" t="n">
         <v>4</v>
@@ -8582,7 +8582,7 @@
         <v>9.321999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>81.5</v>
+        <v>58.5</v>
       </c>
       <c r="D4" t="n">
         <v>45</v>
@@ -8602,10 +8602,10 @@
         <v>9.254</v>
       </c>
       <c r="C5" t="n">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -8622,10 +8622,10 @@
         <v>9.287000000000001</v>
       </c>
       <c r="C6" t="n">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D6" t="n">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -8642,10 +8642,10 @@
         <v>9.609999999999999</v>
       </c>
       <c r="C7" t="n">
+        <v>58</v>
+      </c>
+      <c r="D7" t="n">
         <v>28</v>
-      </c>
-      <c r="D7" t="n">
-        <v>22</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -8662,10 +8662,10 @@
         <v>9.894</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -8682,10 +8682,10 @@
         <v>10.231</v>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D9" t="n">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -8702,10 +8702,10 @@
         <v>10.644</v>
       </c>
       <c r="C10" t="n">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D10" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -8722,10 +8722,10 @@
         <v>11.4075</v>
       </c>
       <c r="C11" t="n">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>37.5</v>
+        <v>60.5</v>
       </c>
       <c r="E11" t="n">
         <v>2</v>
@@ -8742,10 +8742,10 @@
         <v>12.611</v>
       </c>
       <c r="C12" t="n">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="D12" t="n">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="E12" t="n">
         <v>2</v>
@@ -8762,10 +8762,10 @@
         <v>13.576</v>
       </c>
       <c r="C13" t="n">
-        <v>39.33333333333334</v>
+        <v>28</v>
       </c>
       <c r="D13" t="n">
-        <v>67.33333333333333</v>
+        <v>41</v>
       </c>
       <c r="E13" t="n">
         <v>3</v>
@@ -8782,10 +8782,10 @@
         <v>14.1924</v>
       </c>
       <c r="C14" t="n">
-        <v>34</v>
+        <v>29.4</v>
       </c>
       <c r="D14" t="n">
-        <v>61.4</v>
+        <v>65.2</v>
       </c>
       <c r="E14" t="n">
         <v>5</v>
@@ -8802,10 +8802,10 @@
         <v>14.227</v>
       </c>
       <c r="C15" t="n">
-        <v>72.33333333333333</v>
+        <v>58</v>
       </c>
       <c r="D15" t="n">
-        <v>80.33333333333333</v>
+        <v>26.33333333333333</v>
       </c>
       <c r="E15" t="n">
         <v>3</v>
@@ -8822,10 +8822,10 @@
         <v>13.677</v>
       </c>
       <c r="C16" t="n">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="D16" t="n">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -8842,10 +8842,10 @@
         <v>12.7645</v>
       </c>
       <c r="C17" t="n">
-        <v>77</v>
+        <v>57.5</v>
       </c>
       <c r="D17" t="n">
-        <v>43.5</v>
+        <v>73.5</v>
       </c>
       <c r="E17" t="n">
         <v>2</v>
@@ -8862,10 +8862,10 @@
         <v>11.034</v>
       </c>
       <c r="C18" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D18" t="n">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -8882,10 +8882,10 @@
         <v>10.885</v>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D19" t="n">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -8902,10 +8902,10 @@
         <v>11.185</v>
       </c>
       <c r="C20" t="n">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="D20" t="n">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -8922,10 +8922,10 @@
         <v>11.017</v>
       </c>
       <c r="C21" t="n">
-        <v>38</v>
+        <v>11.5</v>
       </c>
       <c r="D21" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E21" t="n">
         <v>2</v>
@@ -8942,10 +8942,10 @@
         <v>10.619</v>
       </c>
       <c r="C22" t="n">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D22" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -8962,10 +8962,10 @@
         <v>9.648999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D23" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -8982,10 +8982,10 @@
         <v>9.109999999999999</v>
       </c>
       <c r="C24" t="n">
-        <v>20.5</v>
+        <v>57</v>
       </c>
       <c r="D24" t="n">
-        <v>47.5</v>
+        <v>59.5</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
@@ -9002,10 +9002,10 @@
         <v>8.752000000000001</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D25" t="n">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -9022,10 +9022,10 @@
         <v>8.245666666666667</v>
       </c>
       <c r="C26" t="n">
-        <v>35.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="D26" t="n">
-        <v>52.16666666666666</v>
+        <v>59.5</v>
       </c>
       <c r="E26" t="n">
         <v>6</v>
@@ -9042,10 +9042,10 @@
         <v>7.596</v>
       </c>
       <c r="C27" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D27" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -9062,10 +9062,10 @@
         <v>6.8515</v>
       </c>
       <c r="C28" t="n">
-        <v>68</v>
+        <v>78.5</v>
       </c>
       <c r="D28" t="n">
-        <v>44.5</v>
+        <v>14.5</v>
       </c>
       <c r="E28" t="n">
         <v>2</v>
@@ -9082,7 +9082,7 @@
         <v>6.198</v>
       </c>
       <c r="C29" t="n">
-        <v>41.2</v>
+        <v>33.2</v>
       </c>
       <c r="D29" t="n">
         <v>52.6</v>
@@ -9102,10 +9102,10 @@
         <v>6.5315</v>
       </c>
       <c r="C30" t="n">
-        <v>45.5</v>
+        <v>74.5</v>
       </c>
       <c r="D30" t="n">
-        <v>58</v>
+        <v>16.5</v>
       </c>
       <c r="E30" t="n">
         <v>2</v>
@@ -9122,10 +9122,10 @@
         <v>6.838</v>
       </c>
       <c r="C31" t="n">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="D31" t="n">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -9142,10 +9142,10 @@
         <v>7.368</v>
       </c>
       <c r="C32" t="n">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E32" t="n">
         <v>1</v>
@@ -9162,10 +9162,10 @@
         <v>8.24</v>
       </c>
       <c r="C33" t="n">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="D33" t="n">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
@@ -9182,10 +9182,10 @@
         <v>9.064</v>
       </c>
       <c r="C34" t="n">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D34" t="n">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="E34" t="n">
         <v>1</v>
@@ -9202,10 +9202,10 @@
         <v>10.407</v>
       </c>
       <c r="C35" t="n">
-        <v>43</v>
+        <v>62.5</v>
       </c>
       <c r="D35" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E35" t="n">
         <v>2</v>
@@ -9222,10 +9222,10 @@
         <v>11.573</v>
       </c>
       <c r="C36" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D36" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
         <v>1</v>
@@ -9242,10 +9242,10 @@
         <v>12.396</v>
       </c>
       <c r="C37" t="n">
-        <v>51.5</v>
+        <v>53.5</v>
       </c>
       <c r="D37" t="n">
-        <v>73</v>
+        <v>65.5</v>
       </c>
       <c r="E37" t="n">
         <v>2</v>
@@ -9262,10 +9262,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C38" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D38" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E38" t="n">
         <v>7</v>
@@ -9282,10 +9282,10 @@
         <v>13.08</v>
       </c>
       <c r="C39" t="n">
-        <v>32.5</v>
+        <v>59.5</v>
       </c>
       <c r="D39" t="n">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E39" t="n">
         <v>2</v>
@@ -9302,10 +9302,10 @@
         <v>12.636</v>
       </c>
       <c r="C40" t="n">
-        <v>38.5</v>
+        <v>55</v>
       </c>
       <c r="D40" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E40" t="n">
         <v>2</v>
@@ -9322,10 +9322,10 @@
         <v>12.187</v>
       </c>
       <c r="C41" t="n">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D41" t="n">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="E41" t="n">
         <v>1</v>
@@ -9342,10 +9342,10 @@
         <v>11.6935</v>
       </c>
       <c r="C42" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D42" t="n">
-        <v>68.5</v>
+        <v>51</v>
       </c>
       <c r="E42" t="n">
         <v>2</v>
@@ -9362,10 +9362,10 @@
         <v>11.071</v>
       </c>
       <c r="C43" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D43" t="n">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="E43" t="n">
         <v>1</v>
@@ -9382,10 +9382,10 @@
         <v>10.163</v>
       </c>
       <c r="C44" t="n">
-        <v>61.5</v>
+        <v>46</v>
       </c>
       <c r="D44" t="n">
-        <v>24.5</v>
+        <v>48</v>
       </c>
       <c r="E44" t="n">
         <v>2</v>
@@ -9402,10 +9402,10 @@
         <v>9.5425</v>
       </c>
       <c r="C45" t="n">
-        <v>92.5</v>
+        <v>75.5</v>
       </c>
       <c r="D45" t="n">
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="E45" t="n">
         <v>2</v>
@@ -9422,10 +9422,10 @@
         <v>9.342000000000001</v>
       </c>
       <c r="C46" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D46" t="n">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="E46" t="n">
         <v>1</v>
@@ -9442,10 +9442,10 @@
         <v>9.249000000000001</v>
       </c>
       <c r="C47" t="n">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="D47" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
@@ -9462,10 +9462,10 @@
         <v>9.146000000000001</v>
       </c>
       <c r="C48" t="n">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D48" t="n">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="E48" t="n">
         <v>1</v>
@@ -9482,10 +9482,10 @@
         <v>9.145</v>
       </c>
       <c r="C49" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D49" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E49" t="n">
         <v>3</v>
@@ -9553,10 +9553,10 @@
         <v>10.2735</v>
       </c>
       <c r="C2" t="n">
-        <v>46.33333333333334</v>
+        <v>51.16666666666666</v>
       </c>
       <c r="D2" t="n">
-        <v>55.33333333333334</v>
+        <v>37.16666666666666</v>
       </c>
       <c r="E2" t="n">
         <v>6</v>
@@ -9573,10 +9573,10 @@
         <v>10.2735</v>
       </c>
       <c r="C3" t="n">
-        <v>46.33333333333334</v>
+        <v>51.16666666666666</v>
       </c>
       <c r="D3" t="n">
-        <v>55.33333333333334</v>
+        <v>37.16666666666666</v>
       </c>
       <c r="E3" t="n">
         <v>6</v>
@@ -9593,10 +9593,10 @@
         <v>10.2735</v>
       </c>
       <c r="C4" t="n">
-        <v>46.33333333333334</v>
+        <v>51.16666666666666</v>
       </c>
       <c r="D4" t="n">
-        <v>55.33333333333334</v>
+        <v>37.16666666666666</v>
       </c>
       <c r="E4" t="n">
         <v>6</v>
@@ -9613,10 +9613,10 @@
         <v>10.2735</v>
       </c>
       <c r="C5" t="n">
-        <v>46.33333333333334</v>
+        <v>51.16666666666666</v>
       </c>
       <c r="D5" t="n">
-        <v>55.33333333333334</v>
+        <v>37.16666666666666</v>
       </c>
       <c r="E5" t="n">
         <v>6</v>
@@ -9633,10 +9633,10 @@
         <v>10.2735</v>
       </c>
       <c r="C6" t="n">
-        <v>46.33333333333334</v>
+        <v>51.16666666666666</v>
       </c>
       <c r="D6" t="n">
-        <v>55.33333333333334</v>
+        <v>37.16666666666666</v>
       </c>
       <c r="E6" t="n">
         <v>6</v>
@@ -9653,10 +9653,10 @@
         <v>10.2735</v>
       </c>
       <c r="C7" t="n">
-        <v>46.33333333333334</v>
+        <v>51.16666666666666</v>
       </c>
       <c r="D7" t="n">
-        <v>55.33333333333334</v>
+        <v>37.16666666666666</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
@@ -9673,10 +9673,10 @@
         <v>9.667249999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>20.5</v>
+        <v>57.75</v>
       </c>
       <c r="D8" t="n">
-        <v>76.75</v>
+        <v>28.75</v>
       </c>
       <c r="E8" t="n">
         <v>4</v>
@@ -9693,10 +9693,10 @@
         <v>9.667249999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>20.5</v>
+        <v>57.75</v>
       </c>
       <c r="D9" t="n">
-        <v>76.75</v>
+        <v>28.75</v>
       </c>
       <c r="E9" t="n">
         <v>4</v>
@@ -9713,10 +9713,10 @@
         <v>9.667249999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>20.5</v>
+        <v>57.75</v>
       </c>
       <c r="D10" t="n">
-        <v>76.75</v>
+        <v>28.75</v>
       </c>
       <c r="E10" t="n">
         <v>4</v>
@@ -9733,10 +9733,10 @@
         <v>9.667249999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>20.5</v>
+        <v>57.75</v>
       </c>
       <c r="D11" t="n">
-        <v>76.75</v>
+        <v>28.75</v>
       </c>
       <c r="E11" t="n">
         <v>4</v>
@@ -9753,7 +9753,7 @@
         <v>9.321999999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>81.5</v>
+        <v>58.5</v>
       </c>
       <c r="D12" t="n">
         <v>45</v>
@@ -9773,7 +9773,7 @@
         <v>9.321999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>81.5</v>
+        <v>58.5</v>
       </c>
       <c r="D13" t="n">
         <v>45</v>
@@ -9793,10 +9793,10 @@
         <v>9.254</v>
       </c>
       <c r="C14" t="n">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -9813,10 +9813,10 @@
         <v>9.287000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D15" t="n">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -9833,10 +9833,10 @@
         <v>9.609999999999999</v>
       </c>
       <c r="C16" t="n">
+        <v>58</v>
+      </c>
+      <c r="D16" t="n">
         <v>28</v>
-      </c>
-      <c r="D16" t="n">
-        <v>22</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -9853,10 +9853,10 @@
         <v>9.894</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -9873,10 +9873,10 @@
         <v>10.231</v>
       </c>
       <c r="C18" t="n">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D18" t="n">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -9893,10 +9893,10 @@
         <v>10.644</v>
       </c>
       <c r="C19" t="n">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D19" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -9913,10 +9913,10 @@
         <v>11.4075</v>
       </c>
       <c r="C20" t="n">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D20" t="n">
-        <v>37.5</v>
+        <v>60.5</v>
       </c>
       <c r="E20" t="n">
         <v>2</v>
@@ -9933,10 +9933,10 @@
         <v>11.4075</v>
       </c>
       <c r="C21" t="n">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D21" t="n">
-        <v>37.5</v>
+        <v>60.5</v>
       </c>
       <c r="E21" t="n">
         <v>2</v>
@@ -9953,10 +9953,10 @@
         <v>12.611</v>
       </c>
       <c r="C22" t="n">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="D22" t="n">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="E22" t="n">
         <v>2</v>
@@ -9973,10 +9973,10 @@
         <v>12.611</v>
       </c>
       <c r="C23" t="n">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="D23" t="n">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="E23" t="n">
         <v>2</v>
@@ -9993,10 +9993,10 @@
         <v>13.576</v>
       </c>
       <c r="C24" t="n">
-        <v>39.33333333333334</v>
+        <v>28</v>
       </c>
       <c r="D24" t="n">
-        <v>67.33333333333333</v>
+        <v>41</v>
       </c>
       <c r="E24" t="n">
         <v>3</v>
@@ -10013,10 +10013,10 @@
         <v>13.576</v>
       </c>
       <c r="C25" t="n">
-        <v>39.33333333333334</v>
+        <v>28</v>
       </c>
       <c r="D25" t="n">
-        <v>67.33333333333333</v>
+        <v>41</v>
       </c>
       <c r="E25" t="n">
         <v>3</v>
@@ -10033,10 +10033,10 @@
         <v>13.576</v>
       </c>
       <c r="C26" t="n">
-        <v>39.33333333333334</v>
+        <v>28</v>
       </c>
       <c r="D26" t="n">
-        <v>67.33333333333333</v>
+        <v>41</v>
       </c>
       <c r="E26" t="n">
         <v>3</v>
@@ -10053,10 +10053,10 @@
         <v>14.1924</v>
       </c>
       <c r="C27" t="n">
-        <v>34</v>
+        <v>29.4</v>
       </c>
       <c r="D27" t="n">
-        <v>61.4</v>
+        <v>65.2</v>
       </c>
       <c r="E27" t="n">
         <v>5</v>
@@ -10073,10 +10073,10 @@
         <v>14.1924</v>
       </c>
       <c r="C28" t="n">
-        <v>34</v>
+        <v>29.4</v>
       </c>
       <c r="D28" t="n">
-        <v>61.4</v>
+        <v>65.2</v>
       </c>
       <c r="E28" t="n">
         <v>5</v>
@@ -10093,10 +10093,10 @@
         <v>14.1924</v>
       </c>
       <c r="C29" t="n">
-        <v>34</v>
+        <v>29.4</v>
       </c>
       <c r="D29" t="n">
-        <v>61.4</v>
+        <v>65.2</v>
       </c>
       <c r="E29" t="n">
         <v>5</v>
@@ -10113,10 +10113,10 @@
         <v>14.1924</v>
       </c>
       <c r="C30" t="n">
-        <v>34</v>
+        <v>29.4</v>
       </c>
       <c r="D30" t="n">
-        <v>61.4</v>
+        <v>65.2</v>
       </c>
       <c r="E30" t="n">
         <v>5</v>
@@ -10133,10 +10133,10 @@
         <v>14.1924</v>
       </c>
       <c r="C31" t="n">
-        <v>34</v>
+        <v>29.4</v>
       </c>
       <c r="D31" t="n">
-        <v>61.4</v>
+        <v>65.2</v>
       </c>
       <c r="E31" t="n">
         <v>5</v>
@@ -10153,10 +10153,10 @@
         <v>14.227</v>
       </c>
       <c r="C32" t="n">
-        <v>72.33333333333333</v>
+        <v>58</v>
       </c>
       <c r="D32" t="n">
-        <v>80.33333333333333</v>
+        <v>26.33333333333333</v>
       </c>
       <c r="E32" t="n">
         <v>3</v>
@@ -10173,10 +10173,10 @@
         <v>14.227</v>
       </c>
       <c r="C33" t="n">
-        <v>72.33333333333333</v>
+        <v>58</v>
       </c>
       <c r="D33" t="n">
-        <v>80.33333333333333</v>
+        <v>26.33333333333333</v>
       </c>
       <c r="E33" t="n">
         <v>3</v>
@@ -10193,10 +10193,10 @@
         <v>14.227</v>
       </c>
       <c r="C34" t="n">
-        <v>72.33333333333333</v>
+        <v>58</v>
       </c>
       <c r="D34" t="n">
-        <v>80.33333333333333</v>
+        <v>26.33333333333333</v>
       </c>
       <c r="E34" t="n">
         <v>3</v>
@@ -10213,10 +10213,10 @@
         <v>13.677</v>
       </c>
       <c r="C35" t="n">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="D35" t="n">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="E35" t="n">
         <v>1</v>
@@ -10233,10 +10233,10 @@
         <v>12.7645</v>
       </c>
       <c r="C36" t="n">
-        <v>77</v>
+        <v>57.5</v>
       </c>
       <c r="D36" t="n">
-        <v>43.5</v>
+        <v>73.5</v>
       </c>
       <c r="E36" t="n">
         <v>2</v>
@@ -10253,10 +10253,10 @@
         <v>12.7645</v>
       </c>
       <c r="C37" t="n">
-        <v>77</v>
+        <v>57.5</v>
       </c>
       <c r="D37" t="n">
-        <v>43.5</v>
+        <v>73.5</v>
       </c>
       <c r="E37" t="n">
         <v>2</v>
@@ -10273,10 +10273,10 @@
         <v>11.034</v>
       </c>
       <c r="C38" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E38" t="n">
         <v>1</v>
@@ -10293,10 +10293,10 @@
         <v>10.885</v>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D39" t="n">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
@@ -10313,10 +10313,10 @@
         <v>11.185</v>
       </c>
       <c r="C40" t="n">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="D40" t="n">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
@@ -10333,10 +10333,10 @@
         <v>11.017</v>
       </c>
       <c r="C41" t="n">
-        <v>38</v>
+        <v>11.5</v>
       </c>
       <c r="D41" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E41" t="n">
         <v>2</v>
@@ -10353,10 +10353,10 @@
         <v>11.017</v>
       </c>
       <c r="C42" t="n">
-        <v>38</v>
+        <v>11.5</v>
       </c>
       <c r="D42" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E42" t="n">
         <v>2</v>
@@ -10373,10 +10373,10 @@
         <v>10.619</v>
       </c>
       <c r="C43" t="n">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D43" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E43" t="n">
         <v>1</v>
@@ -10393,10 +10393,10 @@
         <v>9.648999999999999</v>
       </c>
       <c r="C44" t="n">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D44" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E44" t="n">
         <v>1</v>
@@ -10413,10 +10413,10 @@
         <v>9.109999999999999</v>
       </c>
       <c r="C45" t="n">
-        <v>20.5</v>
+        <v>57</v>
       </c>
       <c r="D45" t="n">
-        <v>47.5</v>
+        <v>59.5</v>
       </c>
       <c r="E45" t="n">
         <v>2</v>
@@ -10433,10 +10433,10 @@
         <v>9.109999999999999</v>
       </c>
       <c r="C46" t="n">
-        <v>20.5</v>
+        <v>57</v>
       </c>
       <c r="D46" t="n">
-        <v>47.5</v>
+        <v>59.5</v>
       </c>
       <c r="E46" t="n">
         <v>2</v>
@@ -10453,10 +10453,10 @@
         <v>8.752000000000001</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D47" t="n">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
@@ -10473,10 +10473,10 @@
         <v>8.245666666666667</v>
       </c>
       <c r="C48" t="n">
-        <v>35.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="D48" t="n">
-        <v>52.16666666666666</v>
+        <v>59.5</v>
       </c>
       <c r="E48" t="n">
         <v>6</v>
@@ -10493,10 +10493,10 @@
         <v>8.245666666666667</v>
       </c>
       <c r="C49" t="n">
-        <v>35.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="D49" t="n">
-        <v>52.16666666666666</v>
+        <v>59.5</v>
       </c>
       <c r="E49" t="n">
         <v>6</v>
@@ -10513,10 +10513,10 @@
         <v>8.245666666666667</v>
       </c>
       <c r="C50" t="n">
-        <v>35.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="D50" t="n">
-        <v>52.16666666666666</v>
+        <v>59.5</v>
       </c>
       <c r="E50" t="n">
         <v>6</v>
@@ -10533,10 +10533,10 @@
         <v>8.245666666666667</v>
       </c>
       <c r="C51" t="n">
-        <v>35.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="D51" t="n">
-        <v>52.16666666666666</v>
+        <v>59.5</v>
       </c>
       <c r="E51" t="n">
         <v>6</v>
@@ -10553,10 +10553,10 @@
         <v>8.245666666666667</v>
       </c>
       <c r="C52" t="n">
-        <v>35.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="D52" t="n">
-        <v>52.16666666666666</v>
+        <v>59.5</v>
       </c>
       <c r="E52" t="n">
         <v>6</v>
@@ -10573,10 +10573,10 @@
         <v>8.245666666666667</v>
       </c>
       <c r="C53" t="n">
-        <v>35.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="D53" t="n">
-        <v>52.16666666666666</v>
+        <v>59.5</v>
       </c>
       <c r="E53" t="n">
         <v>6</v>
@@ -10593,10 +10593,10 @@
         <v>7.596</v>
       </c>
       <c r="C54" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D54" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E54" t="n">
         <v>1</v>
@@ -10613,10 +10613,10 @@
         <v>6.8515</v>
       </c>
       <c r="C55" t="n">
-        <v>68</v>
+        <v>78.5</v>
       </c>
       <c r="D55" t="n">
-        <v>44.5</v>
+        <v>14.5</v>
       </c>
       <c r="E55" t="n">
         <v>2</v>
@@ -10633,10 +10633,10 @@
         <v>6.8515</v>
       </c>
       <c r="C56" t="n">
-        <v>68</v>
+        <v>78.5</v>
       </c>
       <c r="D56" t="n">
-        <v>44.5</v>
+        <v>14.5</v>
       </c>
       <c r="E56" t="n">
         <v>2</v>
@@ -10653,7 +10653,7 @@
         <v>6.198</v>
       </c>
       <c r="C57" t="n">
-        <v>41.2</v>
+        <v>33.2</v>
       </c>
       <c r="D57" t="n">
         <v>52.6</v>
@@ -10673,7 +10673,7 @@
         <v>6.198</v>
       </c>
       <c r="C58" t="n">
-        <v>41.2</v>
+        <v>33.2</v>
       </c>
       <c r="D58" t="n">
         <v>52.6</v>
@@ -10693,7 +10693,7 @@
         <v>6.198</v>
       </c>
       <c r="C59" t="n">
-        <v>41.2</v>
+        <v>33.2</v>
       </c>
       <c r="D59" t="n">
         <v>52.6</v>
@@ -10713,7 +10713,7 @@
         <v>6.198</v>
       </c>
       <c r="C60" t="n">
-        <v>41.2</v>
+        <v>33.2</v>
       </c>
       <c r="D60" t="n">
         <v>52.6</v>
@@ -10733,7 +10733,7 @@
         <v>6.198</v>
       </c>
       <c r="C61" t="n">
-        <v>41.2</v>
+        <v>33.2</v>
       </c>
       <c r="D61" t="n">
         <v>52.6</v>
@@ -10753,10 +10753,10 @@
         <v>6.5315</v>
       </c>
       <c r="C62" t="n">
-        <v>45.5</v>
+        <v>74.5</v>
       </c>
       <c r="D62" t="n">
-        <v>58</v>
+        <v>16.5</v>
       </c>
       <c r="E62" t="n">
         <v>2</v>
@@ -10773,10 +10773,10 @@
         <v>6.5315</v>
       </c>
       <c r="C63" t="n">
-        <v>45.5</v>
+        <v>74.5</v>
       </c>
       <c r="D63" t="n">
-        <v>58</v>
+        <v>16.5</v>
       </c>
       <c r="E63" t="n">
         <v>2</v>
@@ -10793,10 +10793,10 @@
         <v>6.838</v>
       </c>
       <c r="C64" t="n">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="D64" t="n">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="E64" t="n">
         <v>1</v>
@@ -10813,10 +10813,10 @@
         <v>7.368</v>
       </c>
       <c r="C65" t="n">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E65" t="n">
         <v>1</v>
@@ -10833,10 +10833,10 @@
         <v>8.24</v>
       </c>
       <c r="C66" t="n">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="D66" t="n">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="E66" t="n">
         <v>1</v>
@@ -10853,10 +10853,10 @@
         <v>9.064</v>
       </c>
       <c r="C67" t="n">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D67" t="n">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="E67" t="n">
         <v>1</v>
@@ -10873,10 +10873,10 @@
         <v>10.407</v>
       </c>
       <c r="C68" t="n">
-        <v>43</v>
+        <v>62.5</v>
       </c>
       <c r="D68" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E68" t="n">
         <v>2</v>
@@ -10893,10 +10893,10 @@
         <v>10.407</v>
       </c>
       <c r="C69" t="n">
-        <v>43</v>
+        <v>62.5</v>
       </c>
       <c r="D69" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E69" t="n">
         <v>2</v>
@@ -10913,10 +10913,10 @@
         <v>11.573</v>
       </c>
       <c r="C70" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D70" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -10933,10 +10933,10 @@
         <v>12.396</v>
       </c>
       <c r="C71" t="n">
-        <v>51.5</v>
+        <v>53.5</v>
       </c>
       <c r="D71" t="n">
-        <v>73</v>
+        <v>65.5</v>
       </c>
       <c r="E71" t="n">
         <v>2</v>
@@ -10953,10 +10953,10 @@
         <v>12.396</v>
       </c>
       <c r="C72" t="n">
-        <v>51.5</v>
+        <v>53.5</v>
       </c>
       <c r="D72" t="n">
-        <v>73</v>
+        <v>65.5</v>
       </c>
       <c r="E72" t="n">
         <v>2</v>
@@ -10973,10 +10973,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C73" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D73" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E73" t="n">
         <v>7</v>
@@ -10993,10 +10993,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C74" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D74" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E74" t="n">
         <v>7</v>
@@ -11013,10 +11013,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C75" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D75" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E75" t="n">
         <v>7</v>
@@ -11033,10 +11033,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C76" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D76" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E76" t="n">
         <v>7</v>
@@ -11053,10 +11053,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C77" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D77" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E77" t="n">
         <v>7</v>
@@ -11073,10 +11073,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C78" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D78" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E78" t="n">
         <v>7</v>
@@ -11093,10 +11093,10 @@
         <v>13.24671428571429</v>
       </c>
       <c r="C79" t="n">
-        <v>32.57142857142857</v>
+        <v>57.85714285714285</v>
       </c>
       <c r="D79" t="n">
-        <v>52.28571428571428</v>
+        <v>50.71428571428572</v>
       </c>
       <c r="E79" t="n">
         <v>7</v>
@@ -11113,10 +11113,10 @@
         <v>13.08</v>
       </c>
       <c r="C80" t="n">
-        <v>32.5</v>
+        <v>59.5</v>
       </c>
       <c r="D80" t="n">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E80" t="n">
         <v>2</v>
@@ -11133,10 +11133,10 @@
         <v>13.08</v>
       </c>
       <c r="C81" t="n">
-        <v>32.5</v>
+        <v>59.5</v>
       </c>
       <c r="D81" t="n">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E81" t="n">
         <v>2</v>
@@ -11153,10 +11153,10 @@
         <v>12.636</v>
       </c>
       <c r="C82" t="n">
-        <v>38.5</v>
+        <v>55</v>
       </c>
       <c r="D82" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E82" t="n">
         <v>2</v>
@@ -11173,10 +11173,10 @@
         <v>12.636</v>
       </c>
       <c r="C83" t="n">
-        <v>38.5</v>
+        <v>55</v>
       </c>
       <c r="D83" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E83" t="n">
         <v>2</v>
@@ -11193,10 +11193,10 @@
         <v>12.187</v>
       </c>
       <c r="C84" t="n">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D84" t="n">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="E84" t="n">
         <v>1</v>
@@ -11213,10 +11213,10 @@
         <v>11.6935</v>
       </c>
       <c r="C85" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D85" t="n">
-        <v>68.5</v>
+        <v>51</v>
       </c>
       <c r="E85" t="n">
         <v>2</v>
@@ -11233,10 +11233,10 @@
         <v>11.6935</v>
       </c>
       <c r="C86" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D86" t="n">
-        <v>68.5</v>
+        <v>51</v>
       </c>
       <c r="E86" t="n">
         <v>2</v>
@@ -11253,10 +11253,10 @@
         <v>11.071</v>
       </c>
       <c r="C87" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D87" t="n">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="E87" t="n">
         <v>1</v>
@@ -11273,10 +11273,10 @@
         <v>10.163</v>
       </c>
       <c r="C88" t="n">
-        <v>61.5</v>
+        <v>46</v>
       </c>
       <c r="D88" t="n">
-        <v>24.5</v>
+        <v>48</v>
       </c>
       <c r="E88" t="n">
         <v>2</v>
@@ -11293,10 +11293,10 @@
         <v>10.163</v>
       </c>
       <c r="C89" t="n">
-        <v>61.5</v>
+        <v>46</v>
       </c>
       <c r="D89" t="n">
-        <v>24.5</v>
+        <v>48</v>
       </c>
       <c r="E89" t="n">
         <v>2</v>
@@ -11313,10 +11313,10 @@
         <v>9.5425</v>
       </c>
       <c r="C90" t="n">
-        <v>92.5</v>
+        <v>75.5</v>
       </c>
       <c r="D90" t="n">
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="E90" t="n">
         <v>2</v>
@@ -11333,10 +11333,10 @@
         <v>9.5425</v>
       </c>
       <c r="C91" t="n">
-        <v>92.5</v>
+        <v>75.5</v>
       </c>
       <c r="D91" t="n">
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="E91" t="n">
         <v>2</v>
@@ -11353,10 +11353,10 @@
         <v>9.342000000000001</v>
       </c>
       <c r="C92" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D92" t="n">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="E92" t="n">
         <v>1</v>
@@ -11373,10 +11373,10 @@
         <v>9.249000000000001</v>
       </c>
       <c r="C93" t="n">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="D93" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E93" t="n">
         <v>1</v>
@@ -11393,10 +11393,10 @@
         <v>9.146000000000001</v>
       </c>
       <c r="C94" t="n">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D94" t="n">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="E94" t="n">
         <v>1</v>
@@ -11413,10 +11413,10 @@
         <v>9.145</v>
       </c>
       <c r="C95" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D95" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E95" t="n">
         <v>3</v>
@@ -11433,10 +11433,10 @@
         <v>9.145</v>
       </c>
       <c r="C96" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D96" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E96" t="n">
         <v>3</v>
@@ -11453,10 +11453,10 @@
         <v>9.145</v>
       </c>
       <c r="C97" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D97" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E97" t="n">
         <v>3</v>
@@ -11514,10 +11514,10 @@
         <v>10.541</v>
       </c>
       <c r="C2" t="n">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="D2" t="n">
-        <v>89</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -11528,10 +11528,10 @@
         <v>10.472</v>
       </c>
       <c r="C3" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D3" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -11542,10 +11542,10 @@
         <v>10.333</v>
       </c>
       <c r="C4" t="n">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D4" t="n">
-        <v>36</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
@@ -11556,10 +11556,10 @@
         <v>10.216</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D5" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -11570,10 +11570,10 @@
         <v>10.097</v>
       </c>
       <c r="C6" t="n">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D6" t="n">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
@@ -11584,10 +11584,10 @@
         <v>9.981999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D7" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -11598,10 +11598,10 @@
         <v>9.875999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D8" t="n">
-        <v>79</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -11612,10 +11612,10 @@
         <v>9.75</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="D9" t="n">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -11626,10 +11626,10 @@
         <v>9.58</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="D10" t="n">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11">
@@ -11640,10 +11640,10 @@
         <v>9.462999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D11" t="n">
-        <v>79</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -11654,10 +11654,10 @@
         <v>9.353</v>
       </c>
       <c r="C12" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" t="n">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
@@ -11668,10 +11668,10 @@
         <v>9.291</v>
       </c>
       <c r="C13" t="n">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -11682,10 +11682,10 @@
         <v>9.254</v>
       </c>
       <c r="C14" t="n">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>64</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15">
@@ -11696,10 +11696,10 @@
         <v>9.287000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D15" t="n">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16">
@@ -11710,10 +11710,10 @@
         <v>9.609999999999999</v>
       </c>
       <c r="C16" t="n">
+        <v>58</v>
+      </c>
+      <c r="D16" t="n">
         <v>28</v>
-      </c>
-      <c r="D16" t="n">
-        <v>22</v>
       </c>
     </row>
     <row r="17">
@@ -11724,10 +11724,10 @@
         <v>9.894</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -11738,10 +11738,10 @@
         <v>10.231</v>
       </c>
       <c r="C18" t="n">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D18" t="n">
-        <v>27</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19">
@@ -11752,10 +11752,10 @@
         <v>10.644</v>
       </c>
       <c r="C19" t="n">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D19" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20">
@@ -11766,10 +11766,10 @@
         <v>11.168</v>
       </c>
       <c r="C20" t="n">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D20" t="n">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -11780,10 +11780,10 @@
         <v>11.647</v>
       </c>
       <c r="C21" t="n">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="D21" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
@@ -11794,10 +11794,10 @@
         <v>12.115</v>
       </c>
       <c r="C22" t="n">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D22" t="n">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -11808,10 +11808,10 @@
         <v>12.611</v>
       </c>
       <c r="C23" t="n">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="D23" t="n">
-        <v>17</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24">
@@ -11822,10 +11822,10 @@
         <v>13.196</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D24" t="n">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25">
@@ -11836,10 +11836,10 @@
         <v>13.609</v>
       </c>
       <c r="C25" t="n">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="D25" t="n">
-        <v>95</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
@@ -11853,7 +11853,7 @@
         <v>42</v>
       </c>
       <c r="D26" t="n">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27">
@@ -11864,10 +11864,10 @@
         <v>14.111</v>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="D27" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28">
@@ -11878,10 +11878,10 @@
         <v>14.236</v>
       </c>
       <c r="C28" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D28" t="n">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29">
@@ -11892,10 +11892,10 @@
         <v>14.238</v>
       </c>
       <c r="C29" t="n">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="D29" t="n">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30">
@@ -11906,10 +11906,10 @@
         <v>14.186</v>
       </c>
       <c r="C30" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D30" t="n">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31">
@@ -11920,10 +11920,10 @@
         <v>14.191</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D31" t="n">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
@@ -11934,10 +11934,10 @@
         <v>14.325</v>
       </c>
       <c r="C32" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32" t="n">
-        <v>69</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -11948,10 +11948,10 @@
         <v>14.308</v>
       </c>
       <c r="C33" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="D33" t="n">
-        <v>94</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34">
@@ -11962,10 +11962,10 @@
         <v>14.048</v>
       </c>
       <c r="C34" t="n">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D34" t="n">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35">
@@ -11976,10 +11976,10 @@
         <v>13.677</v>
       </c>
       <c r="C35" t="n">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="D35" t="n">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36">
@@ -11990,10 +11990,10 @@
         <v>13.119</v>
       </c>
       <c r="C36" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D36" t="n">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37">
@@ -12004,10 +12004,10 @@
         <v>12.41</v>
       </c>
       <c r="C37" t="n">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="D37" t="n">
-        <v>24</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38">
@@ -12018,10 +12018,10 @@
         <v>11.034</v>
       </c>
       <c r="C38" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39">
@@ -12032,10 +12032,10 @@
         <v>10.885</v>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D39" t="n">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40">
@@ -12046,10 +12046,10 @@
         <v>11.185</v>
       </c>
       <c r="C40" t="n">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="D40" t="n">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41">
@@ -12060,10 +12060,10 @@
         <v>11.063</v>
       </c>
       <c r="C41" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D41" t="n">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
@@ -12074,10 +12074,10 @@
         <v>10.971</v>
       </c>
       <c r="C42" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43">
@@ -12088,10 +12088,10 @@
         <v>10.619</v>
       </c>
       <c r="C43" t="n">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D43" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44">
@@ -12102,10 +12102,10 @@
         <v>9.648999999999999</v>
       </c>
       <c r="C44" t="n">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D44" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45">
@@ -12116,10 +12116,10 @@
         <v>9.185</v>
       </c>
       <c r="C45" t="n">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D45" t="n">
-        <v>67</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46">
@@ -12130,10 +12130,10 @@
         <v>9.035</v>
       </c>
       <c r="C46" t="n">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D46" t="n">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47">
@@ -12144,10 +12144,10 @@
         <v>8.752000000000001</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D47" t="n">
-        <v>91</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48">
@@ -12158,10 +12158,10 @@
         <v>8.298</v>
       </c>
       <c r="C48" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D48" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49">
@@ -12172,10 +12172,10 @@
         <v>8.259</v>
       </c>
       <c r="C49" t="n">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D49" t="n">
-        <v>16</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50">
@@ -12186,10 +12186,10 @@
         <v>8.351000000000001</v>
       </c>
       <c r="C50" t="n">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="D50" t="n">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51">
@@ -12200,10 +12200,10 @@
         <v>8.337</v>
       </c>
       <c r="C51" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D51" t="n">
-        <v>33</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52">
@@ -12214,10 +12214,10 @@
         <v>8.236000000000001</v>
       </c>
       <c r="C52" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D52" t="n">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53">
@@ -12228,10 +12228,10 @@
         <v>7.993</v>
       </c>
       <c r="C53" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D53" t="n">
-        <v>45</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54">
@@ -12242,10 +12242,10 @@
         <v>7.596</v>
       </c>
       <c r="C54" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D54" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55">
@@ -12256,10 +12256,10 @@
         <v>7.163</v>
       </c>
       <c r="C55" t="n">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="D55" t="n">
-        <v>86</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56">
@@ -12270,10 +12270,10 @@
         <v>6.54</v>
       </c>
       <c r="C56" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D56" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57">
@@ -12284,10 +12284,10 @@
         <v>6.17</v>
       </c>
       <c r="C57" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D57" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58">
@@ -12298,10 +12298,10 @@
         <v>5.913</v>
       </c>
       <c r="C58" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D58" t="n">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59">
@@ -12312,10 +12312,10 @@
         <v>5.91</v>
       </c>
       <c r="C59" t="n">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D59" t="n">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60">
@@ -12326,10 +12326,10 @@
         <v>6.477</v>
       </c>
       <c r="C60" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D60" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61">
@@ -12340,10 +12340,10 @@
         <v>6.52</v>
       </c>
       <c r="C61" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D61" t="n">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62">
@@ -12354,10 +12354,10 @@
         <v>6.477</v>
       </c>
       <c r="C62" t="n">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="D62" t="n">
-        <v>77</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63">
@@ -12368,10 +12368,10 @@
         <v>6.586</v>
       </c>
       <c r="C63" t="n">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="D63" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64">
@@ -12382,10 +12382,10 @@
         <v>6.838</v>
       </c>
       <c r="C64" t="n">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="D64" t="n">
-        <v>95</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65">
@@ -12396,10 +12396,10 @@
         <v>7.368</v>
       </c>
       <c r="C65" t="n">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66">
@@ -12410,10 +12410,10 @@
         <v>8.24</v>
       </c>
       <c r="C66" t="n">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="D66" t="n">
-        <v>62</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67">
@@ -12424,10 +12424,10 @@
         <v>9.064</v>
       </c>
       <c r="C67" t="n">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D67" t="n">
-        <v>17</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68">
@@ -12438,10 +12438,10 @@
         <v>10.007</v>
       </c>
       <c r="C68" t="n">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D68" t="n">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69">
@@ -12452,10 +12452,10 @@
         <v>10.807</v>
       </c>
       <c r="C69" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D69" t="n">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70">
@@ -12466,10 +12466,10 @@
         <v>11.573</v>
       </c>
       <c r="C70" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D70" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -12480,10 +12480,10 @@
         <v>12.156</v>
       </c>
       <c r="C71" t="n">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D71" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72">
@@ -12494,10 +12494,10 @@
         <v>12.636</v>
       </c>
       <c r="C72" t="n">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D72" t="n">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73">
@@ -12508,10 +12508,10 @@
         <v>12.981</v>
       </c>
       <c r="C73" t="n">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D73" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74">
@@ -12522,10 +12522,10 @@
         <v>13.298</v>
       </c>
       <c r="C74" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D74" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75">
@@ -12536,10 +12536,10 @@
         <v>13.328</v>
       </c>
       <c r="C75" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D75" t="n">
-        <v>91</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76">
@@ -12550,10 +12550,10 @@
         <v>13.344</v>
       </c>
       <c r="C76" t="n">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="D76" t="n">
-        <v>67</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77">
@@ -12564,10 +12564,10 @@
         <v>13.383</v>
       </c>
       <c r="C77" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D77" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78">
@@ -12578,10 +12578,10 @@
         <v>13.207</v>
       </c>
       <c r="C78" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D78" t="n">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79">
@@ -12592,10 +12592,10 @@
         <v>13.186</v>
       </c>
       <c r="C79" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="D79" t="n">
-        <v>90</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80">
@@ -12606,10 +12606,10 @@
         <v>13.145</v>
       </c>
       <c r="C80" t="n">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D80" t="n">
-        <v>91</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81">
@@ -12620,10 +12620,10 @@
         <v>13.015</v>
       </c>
       <c r="C81" t="n">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D81" t="n">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82">
@@ -12634,10 +12634,10 @@
         <v>12.767</v>
       </c>
       <c r="C82" t="n">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D82" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="83">
@@ -12648,10 +12648,10 @@
         <v>12.505</v>
       </c>
       <c r="C83" t="n">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="D83" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84">
@@ -12662,10 +12662,10 @@
         <v>12.187</v>
       </c>
       <c r="C84" t="n">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D84" t="n">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85">
@@ -12676,10 +12676,10 @@
         <v>11.856</v>
       </c>
       <c r="C85" t="n">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D85" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="86">
@@ -12690,10 +12690,10 @@
         <v>11.531</v>
       </c>
       <c r="C86" t="n">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="D86" t="n">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87">
@@ -12704,10 +12704,10 @@
         <v>11.071</v>
       </c>
       <c r="C87" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D87" t="n">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -12718,10 +12718,10 @@
         <v>10.383</v>
       </c>
       <c r="C88" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D88" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89">
@@ -12732,10 +12732,10 @@
         <v>9.943</v>
       </c>
       <c r="C89" t="n">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="D89" t="n">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90">
@@ -12746,10 +12746,10 @@
         <v>9.65</v>
       </c>
       <c r="C90" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D90" t="n">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91">
@@ -12760,10 +12760,10 @@
         <v>9.435</v>
       </c>
       <c r="C91" t="n">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="D91" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92">
@@ -12774,10 +12774,10 @@
         <v>9.342000000000001</v>
       </c>
       <c r="C92" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D92" t="n">
-        <v>28</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93">
@@ -12788,10 +12788,10 @@
         <v>9.249000000000001</v>
       </c>
       <c r="C93" t="n">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="D93" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="94">
@@ -12802,10 +12802,10 @@
         <v>9.146000000000001</v>
       </c>
       <c r="C94" t="n">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D94" t="n">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95">
@@ -12816,10 +12816,10 @@
         <v>9.145</v>
       </c>
       <c r="C95" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D95" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="96">
@@ -12830,10 +12830,10 @@
         <v>9.140000000000001</v>
       </c>
       <c r="C96" t="n">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D96" t="n">
-        <v>52</v>
+        <v>90</v>
       </c>
     </row>
     <row r="97">
@@ -12844,10 +12844,10 @@
         <v>9.117000000000001</v>
       </c>
       <c r="C97" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D97" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
general stuff and big plotting addition
- global_prio_period in PCTPCAggregator
- better rules for setting prio 2 in PCTPCAggregator
- create_plots to illustrate aggregation of the data
- decompress_df function
- updated example_usage with new functionality
</commit_message>
<xml_diff>
--- a/data/input/example_usage.xlsx
+++ b/data/input/example_usage.xlsx
@@ -8494,7 +8494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8515,123 +8515,63 @@
       </c>
       <c r="C1" s="18" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D1" s="18" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="E1" s="18" t="inlineStr">
-        <is>
           <t>Weights</t>
         </is>
       </c>
-      <c r="F1" s="18" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>25.51066666666667</v>
+        <v>25.108</v>
       </c>
       <c r="B2" t="n">
-        <v>10.2735</v>
+        <v>10.333</v>
       </c>
       <c r="C2" t="n">
-        <v>51.16666666666666</v>
-      </c>
-      <c r="D2" t="n">
-        <v>37.16666666666666</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25.5745</v>
+        <v>25.63925</v>
       </c>
       <c r="B3" t="n">
-        <v>9.667249999999999</v>
+        <v>10.013</v>
       </c>
       <c r="C3" t="n">
-        <v>57.75</v>
-      </c>
-      <c r="D3" t="n">
-        <v>28.75</v>
-      </c>
-      <c r="E3" t="n">
         <v>4</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>26.4745</v>
+        <v>25.40033333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>9.321999999999999</v>
+        <v>9.597666666666667</v>
       </c>
       <c r="C4" t="n">
-        <v>58.5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>45</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>29.223</v>
+        <v>26.4745</v>
       </c>
       <c r="B5" t="n">
-        <v>9.254</v>
+        <v>9.322000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>93</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>28.211</v>
+        <v>28.717</v>
       </c>
       <c r="B6" t="n">
-        <v>9.287000000000001</v>
+        <v>9.2705</v>
       </c>
       <c r="C6" t="n">
-        <v>76</v>
-      </c>
-      <c r="D6" t="n">
-        <v>58</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -8642,15 +8582,6 @@
         <v>9.609999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>58</v>
-      </c>
-      <c r="D7" t="n">
-        <v>28</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8662,156 +8593,84 @@
         <v>9.894</v>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>34.751</v>
+        <v>35.2865</v>
       </c>
       <c r="B9" t="n">
-        <v>10.231</v>
+        <v>10.4375</v>
       </c>
       <c r="C9" t="n">
-        <v>71</v>
-      </c>
-      <c r="D9" t="n">
-        <v>65</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>35.822</v>
+        <v>37.087</v>
       </c>
       <c r="B10" t="n">
-        <v>10.644</v>
+        <v>11.4075</v>
       </c>
       <c r="C10" t="n">
-        <v>52</v>
-      </c>
-      <c r="D10" t="n">
-        <v>65</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>37.087</v>
+        <v>37.879</v>
       </c>
       <c r="B11" t="n">
-        <v>11.4075</v>
+        <v>12.611</v>
       </c>
       <c r="C11" t="n">
-        <v>15</v>
-      </c>
-      <c r="D11" t="n">
-        <v>60.5</v>
-      </c>
-      <c r="E11" t="n">
         <v>2</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>37.879</v>
+        <v>37.733</v>
       </c>
       <c r="B12" t="n">
-        <v>12.611</v>
+        <v>13.196</v>
       </c>
       <c r="C12" t="n">
-        <v>49</v>
-      </c>
-      <c r="D12" t="n">
-        <v>86</v>
-      </c>
-      <c r="E12" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>37.79566666666667</v>
+        <v>37.878</v>
       </c>
       <c r="B13" t="n">
-        <v>13.576</v>
+        <v>13.923</v>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
-      </c>
-      <c r="D13" t="n">
-        <v>41</v>
-      </c>
-      <c r="E13" t="n">
         <v>3</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>37.2936</v>
+        <v>37.296</v>
       </c>
       <c r="B14" t="n">
-        <v>14.1924</v>
+        <v>14.211</v>
       </c>
       <c r="C14" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="D14" t="n">
-        <v>65.2</v>
-      </c>
-      <c r="E14" t="n">
-        <v>5</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>36.464</v>
+        <v>36.46400000000001</v>
       </c>
       <c r="B15" t="n">
         <v>14.227</v>
       </c>
       <c r="C15" t="n">
-        <v>58</v>
-      </c>
-      <c r="D15" t="n">
-        <v>26.33333333333333</v>
-      </c>
-      <c r="E15" t="n">
         <v>3</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -8822,395 +8681,215 @@
         <v>13.677</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D16" t="n">
-        <v>88</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>33.083</v>
+        <v>33.277</v>
       </c>
       <c r="B17" t="n">
-        <v>12.7645</v>
+        <v>13.119</v>
       </c>
       <c r="C17" t="n">
-        <v>57.5</v>
-      </c>
-      <c r="D17" t="n">
-        <v>73.5</v>
-      </c>
-      <c r="E17" t="n">
-        <v>2</v>
-      </c>
-      <c r="F17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>32.311</v>
+        <v>32.889</v>
       </c>
       <c r="B18" t="n">
-        <v>11.034</v>
+        <v>12.41</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
-      </c>
-      <c r="D18" t="n">
-        <v>29</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>33.309</v>
+        <v>32.81</v>
       </c>
       <c r="B19" t="n">
-        <v>10.885</v>
+        <v>10.9595</v>
       </c>
       <c r="C19" t="n">
-        <v>46</v>
-      </c>
-      <c r="D19" t="n">
-        <v>39</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>31.142</v>
+        <v>30.39400000000001</v>
       </c>
       <c r="B20" t="n">
-        <v>11.185</v>
+        <v>11.073</v>
       </c>
       <c r="C20" t="n">
-        <v>36</v>
-      </c>
-      <c r="D20" t="n">
-        <v>40</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>30.02</v>
+        <v>29.168</v>
       </c>
       <c r="B21" t="n">
-        <v>11.017</v>
+        <v>10.619</v>
       </c>
       <c r="C21" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="D21" t="n">
-        <v>36</v>
-      </c>
-      <c r="E21" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>29.168</v>
+        <v>28.189</v>
       </c>
       <c r="B22" t="n">
-        <v>10.619</v>
+        <v>9.648999999999999</v>
       </c>
       <c r="C22" t="n">
-        <v>17</v>
-      </c>
-      <c r="D22" t="n">
-        <v>52</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>28.189</v>
+        <v>26.27066666666667</v>
       </c>
       <c r="B23" t="n">
-        <v>9.648999999999999</v>
+        <v>8.990666666666668</v>
       </c>
       <c r="C23" t="n">
-        <v>18</v>
-      </c>
-      <c r="D23" t="n">
-        <v>79</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>26.5565</v>
+        <v>24.632</v>
       </c>
       <c r="B24" t="n">
-        <v>9.109999999999999</v>
+        <v>8.337</v>
       </c>
       <c r="C24" t="n">
-        <v>57</v>
-      </c>
-      <c r="D24" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E24" t="n">
-        <v>2</v>
-      </c>
-      <c r="F24" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>25.699</v>
+        <v>25.313</v>
       </c>
       <c r="B25" t="n">
-        <v>8.752000000000001</v>
+        <v>7.451666666666667</v>
       </c>
       <c r="C25" t="n">
-        <v>55</v>
-      </c>
-      <c r="D25" t="n">
-        <v>29</v>
-      </c>
-      <c r="E25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>24.8595</v>
+        <v>25.22</v>
       </c>
       <c r="B26" t="n">
-        <v>8.245666666666667</v>
+        <v>6.54</v>
       </c>
       <c r="C26" t="n">
-        <v>35.33333333333334</v>
-      </c>
-      <c r="D26" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E26" t="n">
-        <v>6</v>
-      </c>
-      <c r="F26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>25.492</v>
+        <v>23.99</v>
       </c>
       <c r="B27" t="n">
-        <v>7.596</v>
+        <v>5.91</v>
       </c>
       <c r="C27" t="n">
-        <v>48</v>
-      </c>
-      <c r="D27" t="n">
-        <v>33</v>
-      </c>
-      <c r="E27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>25.0875</v>
+        <v>24.7865</v>
       </c>
       <c r="B28" t="n">
-        <v>6.8515</v>
+        <v>6.4985</v>
       </c>
       <c r="C28" t="n">
-        <v>78.5</v>
-      </c>
-      <c r="D28" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="E28" t="n">
         <v>2</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>24.6124</v>
+        <v>26.1385</v>
       </c>
       <c r="B29" t="n">
-        <v>6.198</v>
+        <v>6.531499999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="D29" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="E29" t="n">
-        <v>5</v>
-      </c>
-      <c r="F29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>26.1385</v>
+        <v>29.084</v>
       </c>
       <c r="B30" t="n">
-        <v>6.5315</v>
+        <v>6.838</v>
       </c>
       <c r="C30" t="n">
-        <v>74.5</v>
-      </c>
-      <c r="D30" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="E30" t="n">
-        <v>2</v>
-      </c>
-      <c r="F30" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>29.084</v>
+        <v>30.866</v>
       </c>
       <c r="B31" t="n">
-        <v>6.838</v>
+        <v>7.368000000000001</v>
       </c>
       <c r="C31" t="n">
-        <v>38</v>
-      </c>
-      <c r="D31" t="n">
-        <v>22</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>30.866</v>
+        <v>32.324</v>
       </c>
       <c r="B32" t="n">
-        <v>7.368</v>
+        <v>8.24</v>
       </c>
       <c r="C32" t="n">
-        <v>90</v>
-      </c>
-      <c r="D32" t="n">
-        <v>15</v>
-      </c>
-      <c r="E32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32.324</v>
+        <v>33.714</v>
       </c>
       <c r="B33" t="n">
-        <v>8.24</v>
+        <v>9.064</v>
       </c>
       <c r="C33" t="n">
-        <v>33</v>
-      </c>
-      <c r="D33" t="n">
-        <v>95</v>
-      </c>
-      <c r="E33" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33.714</v>
+        <v>34.686</v>
       </c>
       <c r="B34" t="n">
-        <v>9.064</v>
+        <v>10.007</v>
       </c>
       <c r="C34" t="n">
-        <v>93</v>
-      </c>
-      <c r="D34" t="n">
-        <v>93</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34.8595</v>
+        <v>35.033</v>
       </c>
       <c r="B35" t="n">
-        <v>10.407</v>
+        <v>10.807</v>
       </c>
       <c r="C35" t="n">
-        <v>62.5</v>
-      </c>
-      <c r="D35" t="n">
-        <v>83</v>
-      </c>
-      <c r="E35" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9222,256 +8901,139 @@
         <v>11.573</v>
       </c>
       <c r="C36" t="n">
-        <v>50</v>
-      </c>
-      <c r="D36" t="n">
-        <v>3</v>
-      </c>
-      <c r="E36" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>35.8475</v>
+        <v>35.737</v>
       </c>
       <c r="B37" t="n">
-        <v>12.396</v>
+        <v>12.156</v>
       </c>
       <c r="C37" t="n">
-        <v>53.5</v>
-      </c>
-      <c r="D37" t="n">
-        <v>65.5</v>
-      </c>
-      <c r="E37" t="n">
-        <v>2</v>
-      </c>
-      <c r="F37" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>35.77685714285715</v>
+        <v>35.8275</v>
       </c>
       <c r="B38" t="n">
-        <v>13.24671428571429</v>
+        <v>12.8085</v>
       </c>
       <c r="C38" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D38" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E38" t="n">
-        <v>7</v>
-      </c>
-      <c r="F38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>34.76300000000001</v>
+        <v>35.86616666666667</v>
       </c>
       <c r="B39" t="n">
-        <v>13.08</v>
+        <v>13.2625</v>
       </c>
       <c r="C39" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="D39" t="n">
-        <v>51</v>
-      </c>
-      <c r="E39" t="n">
-        <v>2</v>
-      </c>
-      <c r="F39" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>33.668</v>
+        <v>34.76300000000001</v>
       </c>
       <c r="B40" t="n">
-        <v>12.636</v>
+        <v>13.08</v>
       </c>
       <c r="C40" t="n">
-        <v>55</v>
-      </c>
-      <c r="D40" t="n">
-        <v>47</v>
-      </c>
-      <c r="E40" t="n">
         <v>2</v>
-      </c>
-      <c r="F40" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>31.966</v>
+        <v>33.668</v>
       </c>
       <c r="B41" t="n">
-        <v>12.187</v>
+        <v>12.636</v>
       </c>
       <c r="C41" t="n">
-        <v>14</v>
-      </c>
-      <c r="D41" t="n">
-        <v>60</v>
-      </c>
-      <c r="E41" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>30.5355</v>
+        <v>31.966</v>
       </c>
       <c r="B42" t="n">
-        <v>11.6935</v>
+        <v>12.187</v>
       </c>
       <c r="C42" t="n">
-        <v>61</v>
-      </c>
-      <c r="D42" t="n">
-        <v>51</v>
-      </c>
-      <c r="E42" t="n">
-        <v>2</v>
-      </c>
-      <c r="F42" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>31.13</v>
+        <v>30.487</v>
       </c>
       <c r="B43" t="n">
-        <v>11.071</v>
+        <v>11.531</v>
       </c>
       <c r="C43" t="n">
-        <v>92</v>
-      </c>
-      <c r="D43" t="n">
-        <v>3</v>
-      </c>
-      <c r="E43" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>28.18</v>
+        <v>31.13</v>
       </c>
       <c r="B44" t="n">
-        <v>10.163</v>
+        <v>11.071</v>
       </c>
       <c r="C44" t="n">
-        <v>46</v>
-      </c>
-      <c r="D44" t="n">
-        <v>48</v>
-      </c>
-      <c r="E44" t="n">
-        <v>2</v>
-      </c>
-      <c r="F44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>27.2805</v>
+        <v>28.18</v>
       </c>
       <c r="B45" t="n">
-        <v>9.5425</v>
+        <v>10.163</v>
       </c>
       <c r="C45" t="n">
-        <v>75.5</v>
-      </c>
-      <c r="D45" t="n">
-        <v>48</v>
-      </c>
-      <c r="E45" t="n">
         <v>2</v>
-      </c>
-      <c r="F45" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>25.961</v>
+        <v>27.2805</v>
       </c>
       <c r="B46" t="n">
-        <v>9.342000000000001</v>
+        <v>9.5425</v>
       </c>
       <c r="C46" t="n">
-        <v>69</v>
-      </c>
-      <c r="D46" t="n">
-        <v>72</v>
-      </c>
-      <c r="E46" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>24.889</v>
+        <v>25.961</v>
       </c>
       <c r="B47" t="n">
-        <v>9.249000000000001</v>
+        <v>9.342000000000001</v>
       </c>
       <c r="C47" t="n">
-        <v>81</v>
-      </c>
-      <c r="D47" t="n">
-        <v>27</v>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>23.864</v>
+        <v>24.3765</v>
       </c>
       <c r="B48" t="n">
-        <v>9.146000000000001</v>
+        <v>9.197500000000002</v>
       </c>
       <c r="C48" t="n">
-        <v>58</v>
-      </c>
-      <c r="D48" t="n">
-        <v>72</v>
-      </c>
-      <c r="E48" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -9482,15 +9044,6 @@
         <v>9.145</v>
       </c>
       <c r="C49" t="n">
-        <v>52</v>
-      </c>
-      <c r="D49" t="n">
-        <v>47</v>
-      </c>
-      <c r="E49" t="n">
-        <v>3</v>
-      </c>
-      <c r="F49" t="n">
         <v>3</v>
       </c>
     </row>
@@ -9505,7 +9058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9526,223 +9079,118 @@
       </c>
       <c r="C1" s="18" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D1" s="18" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="E1" s="18" t="inlineStr">
-        <is>
           <t>Weights</t>
         </is>
       </c>
-      <c r="F1" s="18" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>25.51066666666667</v>
+        <v>25.108</v>
       </c>
       <c r="B2" t="n">
-        <v>10.2735</v>
+        <v>10.333</v>
       </c>
       <c r="C2" t="n">
-        <v>51.16666666666666</v>
-      </c>
-      <c r="D2" t="n">
-        <v>37.16666666666666</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25.51066666666667</v>
+        <v>25.108</v>
       </c>
       <c r="B3" t="n">
-        <v>10.2735</v>
+        <v>10.333</v>
       </c>
       <c r="C3" t="n">
-        <v>51.16666666666666</v>
-      </c>
-      <c r="D3" t="n">
-        <v>37.16666666666666</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>25.51066666666667</v>
+        <v>25.108</v>
       </c>
       <c r="B4" t="n">
-        <v>10.2735</v>
+        <v>10.333</v>
       </c>
       <c r="C4" t="n">
-        <v>51.16666666666666</v>
-      </c>
-      <c r="D4" t="n">
-        <v>37.16666666666666</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>25.51066666666667</v>
+        <v>25.63925</v>
       </c>
       <c r="B5" t="n">
-        <v>10.2735</v>
+        <v>10.013</v>
       </c>
       <c r="C5" t="n">
-        <v>51.16666666666666</v>
-      </c>
-      <c r="D5" t="n">
-        <v>37.16666666666666</v>
-      </c>
-      <c r="E5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>25.51066666666667</v>
+        <v>25.63925</v>
       </c>
       <c r="B6" t="n">
-        <v>10.2735</v>
+        <v>10.013</v>
       </c>
       <c r="C6" t="n">
-        <v>51.16666666666666</v>
-      </c>
-      <c r="D6" t="n">
-        <v>37.16666666666666</v>
-      </c>
-      <c r="E6" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>25.51066666666667</v>
+        <v>25.63925</v>
       </c>
       <c r="B7" t="n">
-        <v>10.2735</v>
+        <v>10.013</v>
       </c>
       <c r="C7" t="n">
-        <v>51.16666666666666</v>
-      </c>
-      <c r="D7" t="n">
-        <v>37.16666666666666</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>25.5745</v>
+        <v>25.63925</v>
       </c>
       <c r="B8" t="n">
-        <v>9.667249999999999</v>
+        <v>10.013</v>
       </c>
       <c r="C8" t="n">
-        <v>57.75</v>
-      </c>
-      <c r="D8" t="n">
-        <v>28.75</v>
-      </c>
-      <c r="E8" t="n">
         <v>4</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>25.5745</v>
+        <v>25.40033333333334</v>
       </c>
       <c r="B9" t="n">
-        <v>9.667249999999999</v>
+        <v>9.597666666666667</v>
       </c>
       <c r="C9" t="n">
-        <v>57.75</v>
-      </c>
-      <c r="D9" t="n">
-        <v>28.75</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>25.5745</v>
+        <v>25.40033333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>9.667249999999999</v>
+        <v>9.597666666666667</v>
       </c>
       <c r="C10" t="n">
-        <v>57.75</v>
-      </c>
-      <c r="D10" t="n">
-        <v>28.75</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>25.5745</v>
+        <v>25.40033333333334</v>
       </c>
       <c r="B11" t="n">
-        <v>9.667249999999999</v>
+        <v>9.597666666666667</v>
       </c>
       <c r="C11" t="n">
-        <v>57.75</v>
-      </c>
-      <c r="D11" t="n">
-        <v>28.75</v>
-      </c>
-      <c r="E11" t="n">
-        <v>4</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -9750,19 +9198,10 @@
         <v>26.4745</v>
       </c>
       <c r="B12" t="n">
-        <v>9.321999999999999</v>
+        <v>9.322000000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>58.5</v>
-      </c>
-      <c r="D12" t="n">
-        <v>45</v>
-      </c>
-      <c r="E12" t="n">
         <v>2</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -9770,59 +9209,32 @@
         <v>26.4745</v>
       </c>
       <c r="B13" t="n">
-        <v>9.321999999999999</v>
+        <v>9.322000000000001</v>
       </c>
       <c r="C13" t="n">
-        <v>58.5</v>
-      </c>
-      <c r="D13" t="n">
-        <v>45</v>
-      </c>
-      <c r="E13" t="n">
         <v>2</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>29.223</v>
+        <v>28.717</v>
       </c>
       <c r="B14" t="n">
-        <v>9.254</v>
+        <v>9.2705</v>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
-      </c>
-      <c r="D14" t="n">
-        <v>93</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>28.211</v>
+        <v>28.717</v>
       </c>
       <c r="B15" t="n">
-        <v>9.287000000000001</v>
+        <v>9.2705</v>
       </c>
       <c r="C15" t="n">
-        <v>76</v>
-      </c>
-      <c r="D15" t="n">
-        <v>58</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -9833,15 +9245,6 @@
         <v>9.609999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>58</v>
-      </c>
-      <c r="D16" t="n">
-        <v>28</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9853,56 +9256,29 @@
         <v>9.894</v>
       </c>
       <c r="C17" t="n">
-        <v>8</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>34.751</v>
+        <v>35.2865</v>
       </c>
       <c r="B18" t="n">
-        <v>10.231</v>
+        <v>10.4375</v>
       </c>
       <c r="C18" t="n">
-        <v>71</v>
-      </c>
-      <c r="D18" t="n">
-        <v>65</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>35.822</v>
+        <v>35.2865</v>
       </c>
       <c r="B19" t="n">
-        <v>10.644</v>
+        <v>10.4375</v>
       </c>
       <c r="C19" t="n">
-        <v>52</v>
-      </c>
-      <c r="D19" t="n">
-        <v>65</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -9913,16 +9289,7 @@
         <v>11.4075</v>
       </c>
       <c r="C20" t="n">
-        <v>15</v>
-      </c>
-      <c r="D20" t="n">
-        <v>60.5</v>
-      </c>
-      <c r="E20" t="n">
         <v>2</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -9933,16 +9300,7 @@
         <v>11.4075</v>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
-      </c>
-      <c r="D21" t="n">
-        <v>60.5</v>
-      </c>
-      <c r="E21" t="n">
         <v>2</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -9953,16 +9311,7 @@
         <v>12.611</v>
       </c>
       <c r="C22" t="n">
-        <v>49</v>
-      </c>
-      <c r="D22" t="n">
-        <v>86</v>
-      </c>
-      <c r="E22" t="n">
         <v>2</v>
-      </c>
-      <c r="F22" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -9973,236 +9322,128 @@
         <v>12.611</v>
       </c>
       <c r="C23" t="n">
-        <v>49</v>
-      </c>
-      <c r="D23" t="n">
-        <v>86</v>
-      </c>
-      <c r="E23" t="n">
         <v>2</v>
-      </c>
-      <c r="F23" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>37.79566666666667</v>
+        <v>37.733</v>
       </c>
       <c r="B24" t="n">
-        <v>13.576</v>
+        <v>13.196</v>
       </c>
       <c r="C24" t="n">
-        <v>28</v>
-      </c>
-      <c r="D24" t="n">
-        <v>41</v>
-      </c>
-      <c r="E24" t="n">
-        <v>3</v>
-      </c>
-      <c r="F24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>37.79566666666667</v>
+        <v>37.878</v>
       </c>
       <c r="B25" t="n">
-        <v>13.576</v>
+        <v>13.923</v>
       </c>
       <c r="C25" t="n">
-        <v>28</v>
-      </c>
-      <c r="D25" t="n">
-        <v>41</v>
-      </c>
-      <c r="E25" t="n">
         <v>3</v>
-      </c>
-      <c r="F25" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>37.79566666666667</v>
+        <v>37.878</v>
       </c>
       <c r="B26" t="n">
-        <v>13.576</v>
+        <v>13.923</v>
       </c>
       <c r="C26" t="n">
-        <v>28</v>
-      </c>
-      <c r="D26" t="n">
-        <v>41</v>
-      </c>
-      <c r="E26" t="n">
         <v>3</v>
-      </c>
-      <c r="F26" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>37.2936</v>
+        <v>37.878</v>
       </c>
       <c r="B27" t="n">
-        <v>14.1924</v>
+        <v>13.923</v>
       </c>
       <c r="C27" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="D27" t="n">
-        <v>65.2</v>
-      </c>
-      <c r="E27" t="n">
-        <v>5</v>
-      </c>
-      <c r="F27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>37.2936</v>
+        <v>37.296</v>
       </c>
       <c r="B28" t="n">
-        <v>14.1924</v>
+        <v>14.211</v>
       </c>
       <c r="C28" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="D28" t="n">
-        <v>65.2</v>
-      </c>
-      <c r="E28" t="n">
-        <v>5</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>37.2936</v>
+        <v>37.296</v>
       </c>
       <c r="B29" t="n">
-        <v>14.1924</v>
+        <v>14.211</v>
       </c>
       <c r="C29" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="D29" t="n">
-        <v>65.2</v>
-      </c>
-      <c r="E29" t="n">
-        <v>5</v>
-      </c>
-      <c r="F29" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>37.2936</v>
+        <v>37.296</v>
       </c>
       <c r="B30" t="n">
-        <v>14.1924</v>
+        <v>14.211</v>
       </c>
       <c r="C30" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="D30" t="n">
-        <v>65.2</v>
-      </c>
-      <c r="E30" t="n">
-        <v>5</v>
-      </c>
-      <c r="F30" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>37.2936</v>
+        <v>37.296</v>
       </c>
       <c r="B31" t="n">
-        <v>14.1924</v>
+        <v>14.211</v>
       </c>
       <c r="C31" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="D31" t="n">
-        <v>65.2</v>
-      </c>
-      <c r="E31" t="n">
-        <v>5</v>
-      </c>
-      <c r="F31" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>36.464</v>
+        <v>36.46400000000001</v>
       </c>
       <c r="B32" t="n">
         <v>14.227</v>
       </c>
       <c r="C32" t="n">
-        <v>58</v>
-      </c>
-      <c r="D32" t="n">
-        <v>26.33333333333333</v>
-      </c>
-      <c r="E32" t="n">
         <v>3</v>
-      </c>
-      <c r="F32" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>36.464</v>
+        <v>36.46400000000001</v>
       </c>
       <c r="B33" t="n">
         <v>14.227</v>
       </c>
       <c r="C33" t="n">
-        <v>58</v>
-      </c>
-      <c r="D33" t="n">
-        <v>26.33333333333333</v>
-      </c>
-      <c r="E33" t="n">
         <v>3</v>
-      </c>
-      <c r="F33" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>36.464</v>
+        <v>36.46400000000001</v>
       </c>
       <c r="B34" t="n">
         <v>14.227</v>
       </c>
       <c r="C34" t="n">
-        <v>58</v>
-      </c>
-      <c r="D34" t="n">
-        <v>26.33333333333333</v>
-      </c>
-      <c r="E34" t="n">
         <v>3</v>
-      </c>
-      <c r="F34" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -10213,156 +9454,84 @@
         <v>13.677</v>
       </c>
       <c r="C35" t="n">
-        <v>10</v>
-      </c>
-      <c r="D35" t="n">
-        <v>88</v>
-      </c>
-      <c r="E35" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>33.083</v>
+        <v>33.277</v>
       </c>
       <c r="B36" t="n">
-        <v>12.7645</v>
+        <v>13.119</v>
       </c>
       <c r="C36" t="n">
-        <v>57.5</v>
-      </c>
-      <c r="D36" t="n">
-        <v>73.5</v>
-      </c>
-      <c r="E36" t="n">
-        <v>2</v>
-      </c>
-      <c r="F36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>33.083</v>
+        <v>32.889</v>
       </c>
       <c r="B37" t="n">
-        <v>12.7645</v>
+        <v>12.41</v>
       </c>
       <c r="C37" t="n">
-        <v>57.5</v>
-      </c>
-      <c r="D37" t="n">
-        <v>73.5</v>
-      </c>
-      <c r="E37" t="n">
-        <v>2</v>
-      </c>
-      <c r="F37" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>32.311</v>
+        <v>32.81</v>
       </c>
       <c r="B38" t="n">
-        <v>11.034</v>
+        <v>10.9595</v>
       </c>
       <c r="C38" t="n">
-        <v>7</v>
-      </c>
-      <c r="D38" t="n">
-        <v>29</v>
-      </c>
-      <c r="E38" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>33.309</v>
+        <v>32.81</v>
       </c>
       <c r="B39" t="n">
-        <v>10.885</v>
+        <v>10.9595</v>
       </c>
       <c r="C39" t="n">
-        <v>46</v>
-      </c>
-      <c r="D39" t="n">
-        <v>39</v>
-      </c>
-      <c r="E39" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>31.142</v>
+        <v>30.39400000000001</v>
       </c>
       <c r="B40" t="n">
-        <v>11.185</v>
+        <v>11.073</v>
       </c>
       <c r="C40" t="n">
-        <v>36</v>
-      </c>
-      <c r="D40" t="n">
-        <v>40</v>
-      </c>
-      <c r="E40" t="n">
-        <v>1</v>
-      </c>
-      <c r="F40" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>30.02</v>
+        <v>30.39400000000001</v>
       </c>
       <c r="B41" t="n">
-        <v>11.017</v>
+        <v>11.073</v>
       </c>
       <c r="C41" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="D41" t="n">
-        <v>36</v>
-      </c>
-      <c r="E41" t="n">
-        <v>2</v>
-      </c>
-      <c r="F41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>30.02</v>
+        <v>30.39400000000001</v>
       </c>
       <c r="B42" t="n">
-        <v>11.017</v>
+        <v>11.073</v>
       </c>
       <c r="C42" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="D42" t="n">
-        <v>36</v>
-      </c>
-      <c r="E42" t="n">
-        <v>2</v>
-      </c>
-      <c r="F42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -10373,15 +9542,6 @@
         <v>10.619</v>
       </c>
       <c r="C43" t="n">
-        <v>17</v>
-      </c>
-      <c r="D43" t="n">
-        <v>52</v>
-      </c>
-      <c r="E43" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10393,356 +9553,194 @@
         <v>9.648999999999999</v>
       </c>
       <c r="C44" t="n">
-        <v>18</v>
-      </c>
-      <c r="D44" t="n">
-        <v>79</v>
-      </c>
-      <c r="E44" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>26.5565</v>
+        <v>26.27066666666667</v>
       </c>
       <c r="B45" t="n">
-        <v>9.109999999999999</v>
+        <v>8.990666666666668</v>
       </c>
       <c r="C45" t="n">
-        <v>57</v>
-      </c>
-      <c r="D45" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E45" t="n">
-        <v>2</v>
-      </c>
-      <c r="F45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>26.5565</v>
+        <v>26.27066666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>9.109999999999999</v>
+        <v>8.990666666666668</v>
       </c>
       <c r="C46" t="n">
-        <v>57</v>
-      </c>
-      <c r="D46" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E46" t="n">
-        <v>2</v>
-      </c>
-      <c r="F46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>25.699</v>
+        <v>26.27066666666667</v>
       </c>
       <c r="B47" t="n">
-        <v>8.752000000000001</v>
+        <v>8.990666666666668</v>
       </c>
       <c r="C47" t="n">
-        <v>55</v>
-      </c>
-      <c r="D47" t="n">
-        <v>29</v>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>24.8595</v>
+        <v>24.632</v>
       </c>
       <c r="B48" t="n">
-        <v>8.245666666666667</v>
+        <v>8.337</v>
       </c>
       <c r="C48" t="n">
-        <v>35.33333333333334</v>
-      </c>
-      <c r="D48" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E48" t="n">
-        <v>6</v>
-      </c>
-      <c r="F48" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>24.8595</v>
+        <v>24.632</v>
       </c>
       <c r="B49" t="n">
-        <v>8.245666666666667</v>
+        <v>8.337</v>
       </c>
       <c r="C49" t="n">
-        <v>35.33333333333334</v>
-      </c>
-      <c r="D49" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E49" t="n">
-        <v>6</v>
-      </c>
-      <c r="F49" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>24.8595</v>
+        <v>24.632</v>
       </c>
       <c r="B50" t="n">
-        <v>8.245666666666667</v>
+        <v>8.337</v>
       </c>
       <c r="C50" t="n">
-        <v>35.33333333333334</v>
-      </c>
-      <c r="D50" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E50" t="n">
-        <v>6</v>
-      </c>
-      <c r="F50" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>24.8595</v>
+        <v>24.632</v>
       </c>
       <c r="B51" t="n">
-        <v>8.245666666666667</v>
+        <v>8.337</v>
       </c>
       <c r="C51" t="n">
-        <v>35.33333333333334</v>
-      </c>
-      <c r="D51" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E51" t="n">
-        <v>6</v>
-      </c>
-      <c r="F51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>24.8595</v>
+        <v>24.632</v>
       </c>
       <c r="B52" t="n">
-        <v>8.245666666666667</v>
+        <v>8.337</v>
       </c>
       <c r="C52" t="n">
-        <v>35.33333333333334</v>
-      </c>
-      <c r="D52" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E52" t="n">
-        <v>6</v>
-      </c>
-      <c r="F52" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>24.8595</v>
+        <v>25.313</v>
       </c>
       <c r="B53" t="n">
-        <v>8.245666666666667</v>
+        <v>7.451666666666667</v>
       </c>
       <c r="C53" t="n">
-        <v>35.33333333333334</v>
-      </c>
-      <c r="D53" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="E53" t="n">
-        <v>6</v>
-      </c>
-      <c r="F53" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>25.492</v>
+        <v>25.313</v>
       </c>
       <c r="B54" t="n">
-        <v>7.596</v>
+        <v>7.451666666666667</v>
       </c>
       <c r="C54" t="n">
-        <v>48</v>
-      </c>
-      <c r="D54" t="n">
-        <v>33</v>
-      </c>
-      <c r="E54" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>25.0875</v>
+        <v>25.313</v>
       </c>
       <c r="B55" t="n">
-        <v>6.8515</v>
+        <v>7.451666666666667</v>
       </c>
       <c r="C55" t="n">
-        <v>78.5</v>
-      </c>
-      <c r="D55" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="E55" t="n">
-        <v>2</v>
-      </c>
-      <c r="F55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>25.0875</v>
+        <v>25.22</v>
       </c>
       <c r="B56" t="n">
-        <v>6.8515</v>
+        <v>6.54</v>
       </c>
       <c r="C56" t="n">
-        <v>78.5</v>
-      </c>
-      <c r="D56" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="E56" t="n">
         <v>2</v>
-      </c>
-      <c r="F56" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>24.6124</v>
+        <v>25.22</v>
       </c>
       <c r="B57" t="n">
-        <v>6.198</v>
+        <v>6.54</v>
       </c>
       <c r="C57" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="D57" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="E57" t="n">
-        <v>5</v>
-      </c>
-      <c r="F57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>24.6124</v>
+        <v>23.99</v>
       </c>
       <c r="B58" t="n">
-        <v>6.198</v>
+        <v>5.91</v>
       </c>
       <c r="C58" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="D58" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="E58" t="n">
-        <v>5</v>
-      </c>
-      <c r="F58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>24.6124</v>
+        <v>23.99</v>
       </c>
       <c r="B59" t="n">
-        <v>6.198</v>
+        <v>5.91</v>
       </c>
       <c r="C59" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="D59" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="E59" t="n">
-        <v>5</v>
-      </c>
-      <c r="F59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>24.6124</v>
+        <v>24.7865</v>
       </c>
       <c r="B60" t="n">
-        <v>6.198</v>
+        <v>6.4985</v>
       </c>
       <c r="C60" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="D60" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="E60" t="n">
-        <v>5</v>
-      </c>
-      <c r="F60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>24.6124</v>
+        <v>24.7865</v>
       </c>
       <c r="B61" t="n">
-        <v>6.198</v>
+        <v>6.4985</v>
       </c>
       <c r="C61" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="D61" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="E61" t="n">
-        <v>5</v>
-      </c>
-      <c r="F61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -10750,19 +9748,10 @@
         <v>26.1385</v>
       </c>
       <c r="B62" t="n">
-        <v>6.5315</v>
+        <v>6.531499999999999</v>
       </c>
       <c r="C62" t="n">
-        <v>74.5</v>
-      </c>
-      <c r="D62" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="E62" t="n">
         <v>2</v>
-      </c>
-      <c r="F62" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -10770,19 +9759,10 @@
         <v>26.1385</v>
       </c>
       <c r="B63" t="n">
-        <v>6.5315</v>
+        <v>6.531499999999999</v>
       </c>
       <c r="C63" t="n">
-        <v>74.5</v>
-      </c>
-      <c r="D63" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="E63" t="n">
         <v>2</v>
-      </c>
-      <c r="F63" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -10793,15 +9773,6 @@
         <v>6.838</v>
       </c>
       <c r="C64" t="n">
-        <v>38</v>
-      </c>
-      <c r="D64" t="n">
-        <v>22</v>
-      </c>
-      <c r="E64" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10810,18 +9781,9 @@
         <v>30.866</v>
       </c>
       <c r="B65" t="n">
-        <v>7.368</v>
+        <v>7.368000000000001</v>
       </c>
       <c r="C65" t="n">
-        <v>90</v>
-      </c>
-      <c r="D65" t="n">
-        <v>15</v>
-      </c>
-      <c r="E65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10833,15 +9795,6 @@
         <v>8.24</v>
       </c>
       <c r="C66" t="n">
-        <v>33</v>
-      </c>
-      <c r="D66" t="n">
-        <v>95</v>
-      </c>
-      <c r="E66" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10853,55 +9806,28 @@
         <v>9.064</v>
       </c>
       <c r="C67" t="n">
-        <v>93</v>
-      </c>
-      <c r="D67" t="n">
-        <v>93</v>
-      </c>
-      <c r="E67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F67" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>34.8595</v>
+        <v>34.686</v>
       </c>
       <c r="B68" t="n">
-        <v>10.407</v>
+        <v>10.007</v>
       </c>
       <c r="C68" t="n">
-        <v>62.5</v>
-      </c>
-      <c r="D68" t="n">
-        <v>83</v>
-      </c>
-      <c r="E68" t="n">
-        <v>2</v>
-      </c>
-      <c r="F68" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>34.8595</v>
+        <v>35.033</v>
       </c>
       <c r="B69" t="n">
-        <v>10.407</v>
+        <v>10.807</v>
       </c>
       <c r="C69" t="n">
-        <v>62.5</v>
-      </c>
-      <c r="D69" t="n">
-        <v>83</v>
-      </c>
-      <c r="E69" t="n">
-        <v>2</v>
-      </c>
-      <c r="F69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10913,196 +9839,106 @@
         <v>11.573</v>
       </c>
       <c r="C70" t="n">
-        <v>50</v>
-      </c>
-      <c r="D70" t="n">
-        <v>3</v>
-      </c>
-      <c r="E70" t="n">
-        <v>1</v>
-      </c>
-      <c r="F70" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>35.8475</v>
+        <v>35.737</v>
       </c>
       <c r="B71" t="n">
-        <v>12.396</v>
+        <v>12.156</v>
       </c>
       <c r="C71" t="n">
-        <v>53.5</v>
-      </c>
-      <c r="D71" t="n">
-        <v>65.5</v>
-      </c>
-      <c r="E71" t="n">
-        <v>2</v>
-      </c>
-      <c r="F71" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>35.8475</v>
+        <v>35.8275</v>
       </c>
       <c r="B72" t="n">
-        <v>12.396</v>
+        <v>12.8085</v>
       </c>
       <c r="C72" t="n">
-        <v>53.5</v>
-      </c>
-      <c r="D72" t="n">
-        <v>65.5</v>
-      </c>
-      <c r="E72" t="n">
         <v>2</v>
-      </c>
-      <c r="F72" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>35.77685714285715</v>
+        <v>35.8275</v>
       </c>
       <c r="B73" t="n">
-        <v>13.24671428571429</v>
+        <v>12.8085</v>
       </c>
       <c r="C73" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D73" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E73" t="n">
-        <v>7</v>
-      </c>
-      <c r="F73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>35.77685714285715</v>
+        <v>35.86616666666667</v>
       </c>
       <c r="B74" t="n">
-        <v>13.24671428571429</v>
+        <v>13.2625</v>
       </c>
       <c r="C74" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D74" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E74" t="n">
-        <v>7</v>
-      </c>
-      <c r="F74" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>35.77685714285715</v>
+        <v>35.86616666666667</v>
       </c>
       <c r="B75" t="n">
-        <v>13.24671428571429</v>
+        <v>13.2625</v>
       </c>
       <c r="C75" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D75" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E75" t="n">
-        <v>7</v>
-      </c>
-      <c r="F75" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>35.77685714285715</v>
+        <v>35.86616666666667</v>
       </c>
       <c r="B76" t="n">
-        <v>13.24671428571429</v>
+        <v>13.2625</v>
       </c>
       <c r="C76" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D76" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E76" t="n">
-        <v>7</v>
-      </c>
-      <c r="F76" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>35.77685714285715</v>
+        <v>35.86616666666667</v>
       </c>
       <c r="B77" t="n">
-        <v>13.24671428571429</v>
+        <v>13.2625</v>
       </c>
       <c r="C77" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D77" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E77" t="n">
-        <v>7</v>
-      </c>
-      <c r="F77" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>35.77685714285715</v>
+        <v>35.86616666666667</v>
       </c>
       <c r="B78" t="n">
-        <v>13.24671428571429</v>
+        <v>13.2625</v>
       </c>
       <c r="C78" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D78" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E78" t="n">
-        <v>7</v>
-      </c>
-      <c r="F78" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>35.77685714285715</v>
+        <v>35.86616666666667</v>
       </c>
       <c r="B79" t="n">
-        <v>13.24671428571429</v>
+        <v>13.2625</v>
       </c>
       <c r="C79" t="n">
-        <v>57.85714285714285</v>
-      </c>
-      <c r="D79" t="n">
-        <v>50.71428571428572</v>
-      </c>
-      <c r="E79" t="n">
-        <v>7</v>
-      </c>
-      <c r="F79" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80">
@@ -11113,16 +9949,7 @@
         <v>13.08</v>
       </c>
       <c r="C80" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="D80" t="n">
-        <v>51</v>
-      </c>
-      <c r="E80" t="n">
         <v>2</v>
-      </c>
-      <c r="F80" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -11133,16 +9960,7 @@
         <v>13.08</v>
       </c>
       <c r="C81" t="n">
-        <v>59.5</v>
-      </c>
-      <c r="D81" t="n">
-        <v>51</v>
-      </c>
-      <c r="E81" t="n">
         <v>2</v>
-      </c>
-      <c r="F81" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -11153,16 +9971,7 @@
         <v>12.636</v>
       </c>
       <c r="C82" t="n">
-        <v>55</v>
-      </c>
-      <c r="D82" t="n">
-        <v>47</v>
-      </c>
-      <c r="E82" t="n">
         <v>2</v>
-      </c>
-      <c r="F82" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -11173,16 +9982,7 @@
         <v>12.636</v>
       </c>
       <c r="C83" t="n">
-        <v>55</v>
-      </c>
-      <c r="D83" t="n">
-        <v>47</v>
-      </c>
-      <c r="E83" t="n">
         <v>2</v>
-      </c>
-      <c r="F83" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -11193,56 +9993,29 @@
         <v>12.187</v>
       </c>
       <c r="C84" t="n">
-        <v>14</v>
-      </c>
-      <c r="D84" t="n">
-        <v>60</v>
-      </c>
-      <c r="E84" t="n">
-        <v>1</v>
-      </c>
-      <c r="F84" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>30.5355</v>
+        <v>30.487</v>
       </c>
       <c r="B85" t="n">
-        <v>11.6935</v>
+        <v>11.531</v>
       </c>
       <c r="C85" t="n">
-        <v>61</v>
-      </c>
-      <c r="D85" t="n">
-        <v>51</v>
-      </c>
-      <c r="E85" t="n">
         <v>2</v>
-      </c>
-      <c r="F85" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>30.5355</v>
+        <v>30.487</v>
       </c>
       <c r="B86" t="n">
-        <v>11.6935</v>
+        <v>11.531</v>
       </c>
       <c r="C86" t="n">
-        <v>61</v>
-      </c>
-      <c r="D86" t="n">
-        <v>51</v>
-      </c>
-      <c r="E86" t="n">
         <v>2</v>
-      </c>
-      <c r="F86" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -11253,15 +10026,6 @@
         <v>11.071</v>
       </c>
       <c r="C87" t="n">
-        <v>92</v>
-      </c>
-      <c r="D87" t="n">
-        <v>3</v>
-      </c>
-      <c r="E87" t="n">
-        <v>1</v>
-      </c>
-      <c r="F87" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11273,16 +10037,7 @@
         <v>10.163</v>
       </c>
       <c r="C88" t="n">
-        <v>46</v>
-      </c>
-      <c r="D88" t="n">
-        <v>48</v>
-      </c>
-      <c r="E88" t="n">
         <v>2</v>
-      </c>
-      <c r="F88" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -11293,16 +10048,7 @@
         <v>10.163</v>
       </c>
       <c r="C89" t="n">
-        <v>46</v>
-      </c>
-      <c r="D89" t="n">
-        <v>48</v>
-      </c>
-      <c r="E89" t="n">
         <v>2</v>
-      </c>
-      <c r="F89" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -11313,16 +10059,7 @@
         <v>9.5425</v>
       </c>
       <c r="C90" t="n">
-        <v>75.5</v>
-      </c>
-      <c r="D90" t="n">
-        <v>48</v>
-      </c>
-      <c r="E90" t="n">
         <v>2</v>
-      </c>
-      <c r="F90" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -11333,16 +10070,7 @@
         <v>9.5425</v>
       </c>
       <c r="C91" t="n">
-        <v>75.5</v>
-      </c>
-      <c r="D91" t="n">
-        <v>48</v>
-      </c>
-      <c r="E91" t="n">
         <v>2</v>
-      </c>
-      <c r="F91" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -11353,56 +10081,29 @@
         <v>9.342000000000001</v>
       </c>
       <c r="C92" t="n">
-        <v>69</v>
-      </c>
-      <c r="D92" t="n">
-        <v>72</v>
-      </c>
-      <c r="E92" t="n">
-        <v>1</v>
-      </c>
-      <c r="F92" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>24.889</v>
+        <v>24.3765</v>
       </c>
       <c r="B93" t="n">
-        <v>9.249000000000001</v>
+        <v>9.197500000000002</v>
       </c>
       <c r="C93" t="n">
-        <v>81</v>
-      </c>
-      <c r="D93" t="n">
-        <v>27</v>
-      </c>
-      <c r="E93" t="n">
-        <v>1</v>
-      </c>
-      <c r="F93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>23.864</v>
+        <v>24.3765</v>
       </c>
       <c r="B94" t="n">
-        <v>9.146000000000001</v>
+        <v>9.197500000000002</v>
       </c>
       <c r="C94" t="n">
-        <v>58</v>
-      </c>
-      <c r="D94" t="n">
-        <v>72</v>
-      </c>
-      <c r="E94" t="n">
-        <v>1</v>
-      </c>
-      <c r="F94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -11413,15 +10114,6 @@
         <v>9.145</v>
       </c>
       <c r="C95" t="n">
-        <v>52</v>
-      </c>
-      <c r="D95" t="n">
-        <v>47</v>
-      </c>
-      <c r="E95" t="n">
-        <v>3</v>
-      </c>
-      <c r="F95" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11433,15 +10125,6 @@
         <v>9.145</v>
       </c>
       <c r="C96" t="n">
-        <v>52</v>
-      </c>
-      <c r="D96" t="n">
-        <v>47</v>
-      </c>
-      <c r="E96" t="n">
-        <v>3</v>
-      </c>
-      <c r="F96" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11453,15 +10136,6 @@
         <v>9.145</v>
       </c>
       <c r="C97" t="n">
-        <v>52</v>
-      </c>
-      <c r="D97" t="n">
-        <v>47</v>
-      </c>
-      <c r="E97" t="n">
-        <v>3</v>
-      </c>
-      <c r="F97" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11476,7 +10150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11495,16 +10169,6 @@
           <t>Temp</t>
         </is>
       </c>
-      <c r="C1" s="18" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D1" s="18" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -11513,12 +10177,6 @@
       <c r="B2" t="n">
         <v>10.541</v>
       </c>
-      <c r="C2" t="n">
-        <v>40</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -11527,12 +10185,6 @@
       <c r="B3" t="n">
         <v>10.472</v>
       </c>
-      <c r="C3" t="n">
-        <v>58</v>
-      </c>
-      <c r="D3" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -11541,12 +10193,6 @@
       <c r="B4" t="n">
         <v>10.333</v>
       </c>
-      <c r="C4" t="n">
-        <v>44</v>
-      </c>
-      <c r="D4" t="n">
-        <v>84</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -11555,12 +10201,6 @@
       <c r="B5" t="n">
         <v>10.216</v>
       </c>
-      <c r="C5" t="n">
-        <v>51</v>
-      </c>
-      <c r="D5" t="n">
-        <v>11</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -11569,12 +10209,6 @@
       <c r="B6" t="n">
         <v>10.097</v>
       </c>
-      <c r="C6" t="n">
-        <v>72</v>
-      </c>
-      <c r="D6" t="n">
-        <v>43</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -11583,12 +10217,6 @@
       <c r="B7" t="n">
         <v>9.981999999999999</v>
       </c>
-      <c r="C7" t="n">
-        <v>42</v>
-      </c>
-      <c r="D7" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -11597,12 +10225,6 @@
       <c r="B8" t="n">
         <v>9.875999999999999</v>
       </c>
-      <c r="C8" t="n">
-        <v>37</v>
-      </c>
-      <c r="D8" t="n">
-        <v>9</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -11611,12 +10233,6 @@
       <c r="B9" t="n">
         <v>9.75</v>
       </c>
-      <c r="C9" t="n">
-        <v>89</v>
-      </c>
-      <c r="D9" t="n">
-        <v>28</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -11625,12 +10241,6 @@
       <c r="B10" t="n">
         <v>9.58</v>
       </c>
-      <c r="C10" t="n">
-        <v>72</v>
-      </c>
-      <c r="D10" t="n">
-        <v>66</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -11639,12 +10249,6 @@
       <c r="B11" t="n">
         <v>9.462999999999999</v>
       </c>
-      <c r="C11" t="n">
-        <v>33</v>
-      </c>
-      <c r="D11" t="n">
-        <v>12</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -11653,12 +10257,6 @@
       <c r="B12" t="n">
         <v>9.353</v>
       </c>
-      <c r="C12" t="n">
-        <v>76</v>
-      </c>
-      <c r="D12" t="n">
-        <v>26</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -11667,12 +10265,6 @@
       <c r="B13" t="n">
         <v>9.291</v>
       </c>
-      <c r="C13" t="n">
-        <v>41</v>
-      </c>
-      <c r="D13" t="n">
-        <v>64</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -11681,12 +10273,6 @@
       <c r="B14" t="n">
         <v>9.254</v>
       </c>
-      <c r="C14" t="n">
-        <v>5</v>
-      </c>
-      <c r="D14" t="n">
-        <v>93</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -11695,12 +10281,6 @@
       <c r="B15" t="n">
         <v>9.287000000000001</v>
       </c>
-      <c r="C15" t="n">
-        <v>76</v>
-      </c>
-      <c r="D15" t="n">
-        <v>58</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -11709,12 +10289,6 @@
       <c r="B16" t="n">
         <v>9.609999999999999</v>
       </c>
-      <c r="C16" t="n">
-        <v>58</v>
-      </c>
-      <c r="D16" t="n">
-        <v>28</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -11723,12 +10297,6 @@
       <c r="B17" t="n">
         <v>9.894</v>
       </c>
-      <c r="C17" t="n">
-        <v>8</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -11737,12 +10305,6 @@
       <c r="B18" t="n">
         <v>10.231</v>
       </c>
-      <c r="C18" t="n">
-        <v>71</v>
-      </c>
-      <c r="D18" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -11751,12 +10313,6 @@
       <c r="B19" t="n">
         <v>10.644</v>
       </c>
-      <c r="C19" t="n">
-        <v>52</v>
-      </c>
-      <c r="D19" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -11765,12 +10321,6 @@
       <c r="B20" t="n">
         <v>11.168</v>
       </c>
-      <c r="C20" t="n">
-        <v>7</v>
-      </c>
-      <c r="D20" t="n">
-        <v>86</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -11779,12 +10329,6 @@
       <c r="B21" t="n">
         <v>11.647</v>
       </c>
-      <c r="C21" t="n">
-        <v>23</v>
-      </c>
-      <c r="D21" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -11793,12 +10337,6 @@
       <c r="B22" t="n">
         <v>12.115</v>
       </c>
-      <c r="C22" t="n">
-        <v>65</v>
-      </c>
-      <c r="D22" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -11807,12 +10345,6 @@
       <c r="B23" t="n">
         <v>12.611</v>
       </c>
-      <c r="C23" t="n">
-        <v>49</v>
-      </c>
-      <c r="D23" t="n">
-        <v>86</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -11821,12 +10353,6 @@
       <c r="B24" t="n">
         <v>13.196</v>
       </c>
-      <c r="C24" t="n">
-        <v>28</v>
-      </c>
-      <c r="D24" t="n">
-        <v>54</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -11835,12 +10361,6 @@
       <c r="B25" t="n">
         <v>13.609</v>
       </c>
-      <c r="C25" t="n">
-        <v>14</v>
-      </c>
-      <c r="D25" t="n">
-        <v>12</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -11849,12 +10369,6 @@
       <c r="B26" t="n">
         <v>13.923</v>
       </c>
-      <c r="C26" t="n">
-        <v>42</v>
-      </c>
-      <c r="D26" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -11863,12 +10377,6 @@
       <c r="B27" t="n">
         <v>14.111</v>
       </c>
-      <c r="C27" t="n">
-        <v>50</v>
-      </c>
-      <c r="D27" t="n">
-        <v>89</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -11877,12 +10385,6 @@
       <c r="B28" t="n">
         <v>14.236</v>
       </c>
-      <c r="C28" t="n">
-        <v>20</v>
-      </c>
-      <c r="D28" t="n">
-        <v>38</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -11891,12 +10393,6 @@
       <c r="B29" t="n">
         <v>14.238</v>
       </c>
-      <c r="C29" t="n">
-        <v>10</v>
-      </c>
-      <c r="D29" t="n">
-        <v>51</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -11905,12 +10401,6 @@
       <c r="B30" t="n">
         <v>14.186</v>
       </c>
-      <c r="C30" t="n">
-        <v>59</v>
-      </c>
-      <c r="D30" t="n">
-        <v>93</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -11919,12 +10409,6 @@
       <c r="B31" t="n">
         <v>14.191</v>
       </c>
-      <c r="C31" t="n">
-        <v>8</v>
-      </c>
-      <c r="D31" t="n">
-        <v>55</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -11933,12 +10417,6 @@
       <c r="B32" t="n">
         <v>14.325</v>
       </c>
-      <c r="C32" t="n">
-        <v>37</v>
-      </c>
-      <c r="D32" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -11947,12 +10425,6 @@
       <c r="B33" t="n">
         <v>14.308</v>
       </c>
-      <c r="C33" t="n">
-        <v>62</v>
-      </c>
-      <c r="D33" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -11961,12 +10433,6 @@
       <c r="B34" t="n">
         <v>14.048</v>
       </c>
-      <c r="C34" t="n">
-        <v>75</v>
-      </c>
-      <c r="D34" t="n">
-        <v>71</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -11975,12 +10441,6 @@
       <c r="B35" t="n">
         <v>13.677</v>
       </c>
-      <c r="C35" t="n">
-        <v>10</v>
-      </c>
-      <c r="D35" t="n">
-        <v>88</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -11989,12 +10449,6 @@
       <c r="B36" t="n">
         <v>13.119</v>
       </c>
-      <c r="C36" t="n">
-        <v>72</v>
-      </c>
-      <c r="D36" t="n">
-        <v>77</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -12003,12 +10457,6 @@
       <c r="B37" t="n">
         <v>12.41</v>
       </c>
-      <c r="C37" t="n">
-        <v>43</v>
-      </c>
-      <c r="D37" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -12017,12 +10465,6 @@
       <c r="B38" t="n">
         <v>11.034</v>
       </c>
-      <c r="C38" t="n">
-        <v>7</v>
-      </c>
-      <c r="D38" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -12031,12 +10473,6 @@
       <c r="B39" t="n">
         <v>10.885</v>
       </c>
-      <c r="C39" t="n">
-        <v>46</v>
-      </c>
-      <c r="D39" t="n">
-        <v>39</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -12045,12 +10481,6 @@
       <c r="B40" t="n">
         <v>11.185</v>
       </c>
-      <c r="C40" t="n">
-        <v>36</v>
-      </c>
-      <c r="D40" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -12059,12 +10489,6 @@
       <c r="B41" t="n">
         <v>11.063</v>
       </c>
-      <c r="C41" t="n">
-        <v>22</v>
-      </c>
-      <c r="D41" t="n">
-        <v>16</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -12073,12 +10497,6 @@
       <c r="B42" t="n">
         <v>10.971</v>
       </c>
-      <c r="C42" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" t="n">
-        <v>56</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -12087,12 +10505,6 @@
       <c r="B43" t="n">
         <v>10.619</v>
       </c>
-      <c r="C43" t="n">
-        <v>17</v>
-      </c>
-      <c r="D43" t="n">
-        <v>52</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -12101,12 +10513,6 @@
       <c r="B44" t="n">
         <v>9.648999999999999</v>
       </c>
-      <c r="C44" t="n">
-        <v>18</v>
-      </c>
-      <c r="D44" t="n">
-        <v>79</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -12115,12 +10521,6 @@
       <c r="B45" t="n">
         <v>9.185</v>
       </c>
-      <c r="C45" t="n">
-        <v>38</v>
-      </c>
-      <c r="D45" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -12129,12 +10529,6 @@
       <c r="B46" t="n">
         <v>9.035</v>
       </c>
-      <c r="C46" t="n">
-        <v>76</v>
-      </c>
-      <c r="D46" t="n">
-        <v>84</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -12143,12 +10537,6 @@
       <c r="B47" t="n">
         <v>8.752000000000001</v>
       </c>
-      <c r="C47" t="n">
-        <v>55</v>
-      </c>
-      <c r="D47" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -12157,12 +10545,6 @@
       <c r="B48" t="n">
         <v>8.298</v>
       </c>
-      <c r="C48" t="n">
-        <v>67</v>
-      </c>
-      <c r="D48" t="n">
-        <v>8</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -12171,12 +10553,6 @@
       <c r="B49" t="n">
         <v>8.259</v>
       </c>
-      <c r="C49" t="n">
-        <v>44</v>
-      </c>
-      <c r="D49" t="n">
-        <v>94</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -12185,12 +10561,6 @@
       <c r="B50" t="n">
         <v>8.351000000000001</v>
       </c>
-      <c r="C50" t="n">
-        <v>5</v>
-      </c>
-      <c r="D50" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -12199,12 +10569,6 @@
       <c r="B51" t="n">
         <v>8.337</v>
       </c>
-      <c r="C51" t="n">
-        <v>10</v>
-      </c>
-      <c r="D51" t="n">
-        <v>71</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -12213,12 +10577,6 @@
       <c r="B52" t="n">
         <v>8.236000000000001</v>
       </c>
-      <c r="C52" t="n">
-        <v>32</v>
-      </c>
-      <c r="D52" t="n">
-        <v>68</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -12227,12 +10585,6 @@
       <c r="B53" t="n">
         <v>7.993</v>
       </c>
-      <c r="C53" t="n">
-        <v>54</v>
-      </c>
-      <c r="D53" t="n">
-        <v>81</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -12241,12 +10593,6 @@
       <c r="B54" t="n">
         <v>7.596</v>
       </c>
-      <c r="C54" t="n">
-        <v>48</v>
-      </c>
-      <c r="D54" t="n">
-        <v>33</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -12255,12 +10601,6 @@
       <c r="B55" t="n">
         <v>7.163</v>
       </c>
-      <c r="C55" t="n">
-        <v>90</v>
-      </c>
-      <c r="D55" t="n">
-        <v>12</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -12269,12 +10609,6 @@
       <c r="B56" t="n">
         <v>6.54</v>
       </c>
-      <c r="C56" t="n">
-        <v>67</v>
-      </c>
-      <c r="D56" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -12283,12 +10617,6 @@
       <c r="B57" t="n">
         <v>6.17</v>
       </c>
-      <c r="C57" t="n">
-        <v>8</v>
-      </c>
-      <c r="D57" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -12297,12 +10625,6 @@
       <c r="B58" t="n">
         <v>5.913</v>
       </c>
-      <c r="C58" t="n">
-        <v>71</v>
-      </c>
-      <c r="D58" t="n">
-        <v>88</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -12311,12 +10633,6 @@
       <c r="B59" t="n">
         <v>5.91</v>
       </c>
-      <c r="C59" t="n">
-        <v>26</v>
-      </c>
-      <c r="D59" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -12325,12 +10641,6 @@
       <c r="B60" t="n">
         <v>6.477</v>
       </c>
-      <c r="C60" t="n">
-        <v>40</v>
-      </c>
-      <c r="D60" t="n">
-        <v>61</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -12339,12 +10649,6 @@
       <c r="B61" t="n">
         <v>6.52</v>
       </c>
-      <c r="C61" t="n">
-        <v>21</v>
-      </c>
-      <c r="D61" t="n">
-        <v>64</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -12353,12 +10657,6 @@
       <c r="B62" t="n">
         <v>6.477</v>
       </c>
-      <c r="C62" t="n">
-        <v>55</v>
-      </c>
-      <c r="D62" t="n">
-        <v>9</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -12367,12 +10665,6 @@
       <c r="B63" t="n">
         <v>6.586</v>
       </c>
-      <c r="C63" t="n">
-        <v>94</v>
-      </c>
-      <c r="D63" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -12381,12 +10673,6 @@
       <c r="B64" t="n">
         <v>6.838</v>
       </c>
-      <c r="C64" t="n">
-        <v>38</v>
-      </c>
-      <c r="D64" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -12395,12 +10681,6 @@
       <c r="B65" t="n">
         <v>7.368</v>
       </c>
-      <c r="C65" t="n">
-        <v>90</v>
-      </c>
-      <c r="D65" t="n">
-        <v>15</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -12409,12 +10689,6 @@
       <c r="B66" t="n">
         <v>8.24</v>
       </c>
-      <c r="C66" t="n">
-        <v>33</v>
-      </c>
-      <c r="D66" t="n">
-        <v>95</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -12423,12 +10697,6 @@
       <c r="B67" t="n">
         <v>9.064</v>
       </c>
-      <c r="C67" t="n">
-        <v>93</v>
-      </c>
-      <c r="D67" t="n">
-        <v>93</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -12437,12 +10705,6 @@
       <c r="B68" t="n">
         <v>10.007</v>
       </c>
-      <c r="C68" t="n">
-        <v>84</v>
-      </c>
-      <c r="D68" t="n">
-        <v>94</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -12451,12 +10713,6 @@
       <c r="B69" t="n">
         <v>10.807</v>
       </c>
-      <c r="C69" t="n">
-        <v>41</v>
-      </c>
-      <c r="D69" t="n">
-        <v>72</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -12465,12 +10721,6 @@
       <c r="B70" t="n">
         <v>11.573</v>
       </c>
-      <c r="C70" t="n">
-        <v>50</v>
-      </c>
-      <c r="D70" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -12479,12 +10729,6 @@
       <c r="B71" t="n">
         <v>12.156</v>
       </c>
-      <c r="C71" t="n">
-        <v>45</v>
-      </c>
-      <c r="D71" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -12493,12 +10737,6 @@
       <c r="B72" t="n">
         <v>12.636</v>
       </c>
-      <c r="C72" t="n">
-        <v>62</v>
-      </c>
-      <c r="D72" t="n">
-        <v>74</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -12507,12 +10745,6 @@
       <c r="B73" t="n">
         <v>12.981</v>
       </c>
-      <c r="C73" t="n">
-        <v>77</v>
-      </c>
-      <c r="D73" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -12521,12 +10753,6 @@
       <c r="B74" t="n">
         <v>13.298</v>
       </c>
-      <c r="C74" t="n">
-        <v>27</v>
-      </c>
-      <c r="D74" t="n">
-        <v>32</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -12535,12 +10761,6 @@
       <c r="B75" t="n">
         <v>13.328</v>
       </c>
-      <c r="C75" t="n">
-        <v>75</v>
-      </c>
-      <c r="D75" t="n">
-        <v>63</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -12549,12 +10769,6 @@
       <c r="B76" t="n">
         <v>13.344</v>
       </c>
-      <c r="C76" t="n">
-        <v>86</v>
-      </c>
-      <c r="D76" t="n">
-        <v>86</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -12563,12 +10777,6 @@
       <c r="B77" t="n">
         <v>13.383</v>
       </c>
-      <c r="C77" t="n">
-        <v>20</v>
-      </c>
-      <c r="D77" t="n">
-        <v>43</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -12577,12 +10785,6 @@
       <c r="B78" t="n">
         <v>13.207</v>
       </c>
-      <c r="C78" t="n">
-        <v>27</v>
-      </c>
-      <c r="D78" t="n">
-        <v>61</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -12591,12 +10793,6 @@
       <c r="B79" t="n">
         <v>13.186</v>
       </c>
-      <c r="C79" t="n">
-        <v>93</v>
-      </c>
-      <c r="D79" t="n">
-        <v>43</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -12605,12 +10801,6 @@
       <c r="B80" t="n">
         <v>13.145</v>
       </c>
-      <c r="C80" t="n">
-        <v>70</v>
-      </c>
-      <c r="D80" t="n">
-        <v>8</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -12619,12 +10809,6 @@
       <c r="B81" t="n">
         <v>13.015</v>
       </c>
-      <c r="C81" t="n">
-        <v>49</v>
-      </c>
-      <c r="D81" t="n">
-        <v>94</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -12633,12 +10817,6 @@
       <c r="B82" t="n">
         <v>12.767</v>
       </c>
-      <c r="C82" t="n">
-        <v>36</v>
-      </c>
-      <c r="D82" t="n">
-        <v>49</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -12647,12 +10825,6 @@
       <c r="B83" t="n">
         <v>12.505</v>
       </c>
-      <c r="C83" t="n">
-        <v>74</v>
-      </c>
-      <c r="D83" t="n">
-        <v>45</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -12661,12 +10833,6 @@
       <c r="B84" t="n">
         <v>12.187</v>
       </c>
-      <c r="C84" t="n">
-        <v>14</v>
-      </c>
-      <c r="D84" t="n">
-        <v>60</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -12675,12 +10841,6 @@
       <c r="B85" t="n">
         <v>11.856</v>
       </c>
-      <c r="C85" t="n">
-        <v>50</v>
-      </c>
-      <c r="D85" t="n">
-        <v>67</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -12689,12 +10849,6 @@
       <c r="B86" t="n">
         <v>11.531</v>
       </c>
-      <c r="C86" t="n">
-        <v>72</v>
-      </c>
-      <c r="D86" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -12703,12 +10857,6 @@
       <c r="B87" t="n">
         <v>11.071</v>
       </c>
-      <c r="C87" t="n">
-        <v>92</v>
-      </c>
-      <c r="D87" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -12717,12 +10865,6 @@
       <c r="B88" t="n">
         <v>10.383</v>
       </c>
-      <c r="C88" t="n">
-        <v>53</v>
-      </c>
-      <c r="D88" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -12731,12 +10873,6 @@
       <c r="B89" t="n">
         <v>9.943</v>
       </c>
-      <c r="C89" t="n">
-        <v>39</v>
-      </c>
-      <c r="D89" t="n">
-        <v>77</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -12745,12 +10881,6 @@
       <c r="B90" t="n">
         <v>9.65</v>
       </c>
-      <c r="C90" t="n">
-        <v>95</v>
-      </c>
-      <c r="D90" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -12759,12 +10889,6 @@
       <c r="B91" t="n">
         <v>9.435</v>
       </c>
-      <c r="C91" t="n">
-        <v>56</v>
-      </c>
-      <c r="D91" t="n">
-        <v>31</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -12773,12 +10897,6 @@
       <c r="B92" t="n">
         <v>9.342000000000001</v>
       </c>
-      <c r="C92" t="n">
-        <v>69</v>
-      </c>
-      <c r="D92" t="n">
-        <v>72</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -12787,12 +10905,6 @@
       <c r="B93" t="n">
         <v>9.249000000000001</v>
       </c>
-      <c r="C93" t="n">
-        <v>81</v>
-      </c>
-      <c r="D93" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -12801,12 +10913,6 @@
       <c r="B94" t="n">
         <v>9.146000000000001</v>
       </c>
-      <c r="C94" t="n">
-        <v>58</v>
-      </c>
-      <c r="D94" t="n">
-        <v>72</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -12815,12 +10921,6 @@
       <c r="B95" t="n">
         <v>9.145</v>
       </c>
-      <c r="C95" t="n">
-        <v>52</v>
-      </c>
-      <c r="D95" t="n">
-        <v>47</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -12829,12 +10929,6 @@
       <c r="B96" t="n">
         <v>9.140000000000001</v>
       </c>
-      <c r="C96" t="n">
-        <v>33</v>
-      </c>
-      <c r="D96" t="n">
-        <v>90</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -12842,12 +10936,6 @@
       </c>
       <c r="B97" t="n">
         <v>9.117000000000001</v>
-      </c>
-      <c r="C97" t="n">
-        <v>37</v>
-      </c>
-      <c r="D97" t="n">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>